<commit_message>
final updatation of gantt chart in excel sheet
</commit_message>
<xml_diff>
--- a/Gantt chart.xlsx
+++ b/Gantt chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pranj\software-tech-ass\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ACCA10F-9F17-4406-9FB4-62F0345B1706}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F553B48-5D24-4F2F-A95E-42EFA6E0D0CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,6 +27,7 @@
     <definedName name="TitleRegion..BO60">#REF!</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -39,15 +40,12 @@
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="72">
   <si>
     <t>ACTIVITY</t>
   </si>
@@ -236,13 +234,40 @@
   </si>
   <si>
     <t>Days</t>
+  </si>
+  <si>
+    <t>Update and review everything</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plan Duratioon </t>
+  </si>
+  <si>
+    <t>Actual Duration</t>
+  </si>
+  <si>
+    <t>According to Plan</t>
+  </si>
+  <si>
+    <t>Delay</t>
+  </si>
+  <si>
+    <t>(lining)</t>
+  </si>
+  <si>
+    <t>Any color</t>
+  </si>
+  <si>
+    <t>lining + color</t>
+  </si>
+  <si>
+    <t>lining after color</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1" tint="0.24994659260841701"/>
@@ -357,8 +382,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1" tint="0.24994659260841701"/>
+      <name val="Corbel"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
   </fonts>
-  <fills count="22">
+  <fills count="29">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -420,24 +453,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF002060"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -484,8 +499,68 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightUp">
+        <fgColor theme="7"/>
+        <bgColor rgb="FFFF0000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightUp">
+        <fgColor theme="7"/>
+        <bgColor rgb="FF002060"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightUp">
+        <fgColor theme="7"/>
+        <bgColor rgb="FF00B050"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightUp">
+        <fgColor theme="7"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightUp">
+        <fgColor theme="7"/>
+        <bgColor rgb="FFC00000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightUp">
+        <fgColor theme="7"/>
+        <bgColor rgb="FFFFC000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightUp">
+        <fgColor theme="7"/>
+        <bgColor rgb="FF0070C0"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -576,6 +651,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
@@ -634,7 +724,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -686,68 +776,101 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="6" fillId="19" borderId="2" xfId="3" applyFill="1">
+    <xf numFmtId="3" fontId="6" fillId="16" borderId="2" xfId="3" applyFill="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" xfId="11" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="3" xfId="15" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" xfId="9" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="3" xfId="15" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="15" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="10" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" xfId="11" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" xfId="9" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="2" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="2" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" xfId="10" applyFill="1">
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" xfId="10" applyFill="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="2" xfId="10" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="2" xfId="10" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="5" xfId="10" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="5" xfId="10" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="10" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="3" xfId="15" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="3" xfId="15" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="3" xfId="15" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="3" xfId="15" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="8" xfId="15" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="26" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="28" borderId="8" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="0" borderId="0" xfId="3" applyBorder="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -1032,73 +1155,76 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BB98ED6-7229-4B86-9462-BCFB5BEE7D24}">
-  <dimension ref="A1:BN58"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:BN59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="51" zoomScaleNormal="25" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="72" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AO44" sqref="AO44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="53.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="66" width="4.77734375" customWidth="1"/>
+    <col min="1" max="1" width="53.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="66" width="4.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:66" x14ac:dyDescent="0.3">
-      <c r="A1" s="32" t="s">
+    <row r="1" spans="1:66" x14ac:dyDescent="0.25">
+      <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="34" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="34" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="34" t="s">
+      <c r="B1" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="36" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="34" t="s">
+      <c r="E1" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="36" t="s">
+      <c r="F1" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="31" t="s">
+      <c r="G1" s="33" t="s">
         <v>62</v>
       </c>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
-      <c r="L1" s="31"/>
-      <c r="M1" s="31"/>
-      <c r="N1" s="31"/>
-      <c r="O1" s="31"/>
-      <c r="P1" s="31"/>
-      <c r="Q1" s="31"/>
-      <c r="R1" s="31"/>
-      <c r="S1" s="31"/>
-      <c r="T1" s="31"/>
-      <c r="U1" s="31"/>
-      <c r="V1" s="31"/>
-      <c r="W1" s="31"/>
-      <c r="X1" s="31"/>
-      <c r="Y1" s="31"/>
-      <c r="Z1" s="31"/>
-      <c r="AA1" s="31"/>
-      <c r="AB1" s="31"/>
-      <c r="AC1" s="31"/>
-      <c r="AD1" s="31"/>
-      <c r="AE1" s="31"/>
-      <c r="AF1" s="31"/>
-      <c r="AG1" s="31"/>
-      <c r="AH1" s="31"/>
-      <c r="AI1" s="31"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="33"/>
+      <c r="N1" s="33"/>
+      <c r="O1" s="33"/>
+      <c r="P1" s="33"/>
+      <c r="Q1" s="33"/>
+      <c r="R1" s="33"/>
+      <c r="S1" s="33"/>
+      <c r="T1" s="33"/>
+      <c r="U1" s="33"/>
+      <c r="V1" s="33"/>
+      <c r="W1" s="33"/>
+      <c r="X1" s="33"/>
+      <c r="Y1" s="33"/>
+      <c r="Z1" s="33"/>
+      <c r="AA1" s="33"/>
+      <c r="AB1" s="33"/>
+      <c r="AC1" s="33"/>
+      <c r="AD1" s="33"/>
+      <c r="AE1" s="33"/>
+      <c r="AF1" s="33"/>
+      <c r="AG1" s="33"/>
+      <c r="AH1" s="33"/>
+      <c r="AI1" s="33"/>
       <c r="AJ1" s="2"/>
       <c r="AK1" s="2"/>
       <c r="AL1" s="2"/>
@@ -1131,142 +1257,142 @@
       <c r="BM1" s="2"/>
       <c r="BN1" s="2"/>
     </row>
-    <row r="2" spans="1:66" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="33"/>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="30">
-        <v>1</v>
-      </c>
-      <c r="H2" s="30">
-        <v>2</v>
-      </c>
-      <c r="I2" s="30">
+    <row r="2" spans="1:66" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="35"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="27">
+        <v>1</v>
+      </c>
+      <c r="H2" s="27">
+        <v>2</v>
+      </c>
+      <c r="I2" s="27">
         <v>3</v>
       </c>
-      <c r="J2" s="30">
+      <c r="J2" s="27">
         <v>4</v>
       </c>
-      <c r="K2" s="30">
+      <c r="K2" s="27">
         <v>5</v>
       </c>
-      <c r="L2" s="30">
+      <c r="L2" s="27">
         <v>6</v>
       </c>
-      <c r="M2" s="30">
+      <c r="M2" s="27">
         <v>7</v>
       </c>
-      <c r="N2" s="30">
+      <c r="N2" s="27">
         <v>8</v>
       </c>
-      <c r="O2" s="30">
+      <c r="O2" s="27">
         <v>9</v>
       </c>
-      <c r="P2" s="30">
+      <c r="P2" s="27">
         <v>10</v>
       </c>
-      <c r="Q2" s="30">
+      <c r="Q2" s="27">
         <v>11</v>
       </c>
-      <c r="R2" s="30">
+      <c r="R2" s="27">
         <v>12</v>
       </c>
-      <c r="S2" s="30">
+      <c r="S2" s="27">
         <v>13</v>
       </c>
-      <c r="T2" s="30">
+      <c r="T2" s="27">
         <v>14</v>
       </c>
-      <c r="U2" s="30">
+      <c r="U2" s="27">
         <v>15</v>
       </c>
-      <c r="V2" s="30">
+      <c r="V2" s="27">
         <v>16</v>
       </c>
-      <c r="W2" s="30">
+      <c r="W2" s="27">
         <v>17</v>
       </c>
-      <c r="X2" s="30">
+      <c r="X2" s="27">
         <v>18</v>
       </c>
-      <c r="Y2" s="30">
+      <c r="Y2" s="27">
         <v>19</v>
       </c>
-      <c r="Z2" s="30">
+      <c r="Z2" s="27">
         <v>20</v>
       </c>
-      <c r="AA2" s="30">
+      <c r="AA2" s="27">
         <v>21</v>
       </c>
-      <c r="AB2" s="30">
+      <c r="AB2" s="27">
         <v>22</v>
       </c>
-      <c r="AC2" s="30">
+      <c r="AC2" s="27">
         <v>23</v>
       </c>
-      <c r="AD2" s="30">
+      <c r="AD2" s="27">
         <v>24</v>
       </c>
-      <c r="AE2" s="30">
+      <c r="AE2" s="27">
         <v>25</v>
       </c>
-      <c r="AF2" s="30">
+      <c r="AF2" s="27">
         <v>26</v>
       </c>
-      <c r="AG2" s="30">
+      <c r="AG2" s="27">
         <v>27</v>
       </c>
-      <c r="AH2" s="30">
+      <c r="AH2" s="27">
         <v>28</v>
       </c>
-      <c r="AI2" s="30">
+      <c r="AI2" s="27">
         <v>29</v>
       </c>
-      <c r="AJ2" s="1"/>
-      <c r="AK2" s="1"/>
-      <c r="AL2" s="1"/>
-      <c r="AM2" s="1"/>
-      <c r="AN2" s="1"/>
-      <c r="AO2" s="1"/>
-      <c r="AP2" s="1"/>
-      <c r="AQ2" s="1"/>
-      <c r="AR2" s="1"/>
-      <c r="AS2" s="1"/>
-      <c r="AT2" s="1"/>
-      <c r="AU2" s="1"/>
-      <c r="AV2" s="1"/>
-      <c r="AW2" s="1"/>
-      <c r="AX2" s="1"/>
-      <c r="AY2" s="1"/>
-      <c r="AZ2" s="1"/>
-      <c r="BA2" s="1"/>
-      <c r="BB2" s="1"/>
-      <c r="BC2" s="1"/>
-      <c r="BD2" s="1"/>
-      <c r="BE2" s="1"/>
-      <c r="BF2" s="1"/>
-      <c r="BG2" s="1"/>
-      <c r="BH2" s="1"/>
-      <c r="BI2" s="1"/>
-      <c r="BJ2" s="1"/>
-      <c r="BK2" s="1"/>
-      <c r="BL2" s="1"/>
-      <c r="BM2" s="1"/>
-      <c r="BN2" s="1"/>
-    </row>
-    <row r="3" spans="1:66" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AJ2" s="48"/>
+      <c r="AK2" s="48"/>
+      <c r="AL2" s="48"/>
+      <c r="AM2" s="48"/>
+      <c r="AN2" s="48"/>
+      <c r="AO2" s="48"/>
+      <c r="AP2" s="48"/>
+      <c r="AQ2" s="48"/>
+      <c r="AR2" s="48"/>
+      <c r="AS2" s="48"/>
+      <c r="AT2" s="48"/>
+      <c r="AU2" s="48"/>
+      <c r="AV2" s="48"/>
+      <c r="AW2" s="48"/>
+      <c r="AX2" s="48"/>
+      <c r="AY2" s="48"/>
+      <c r="AZ2" s="48"/>
+      <c r="BA2" s="48"/>
+      <c r="BB2" s="48"/>
+      <c r="BC2" s="48"/>
+      <c r="BD2" s="48"/>
+      <c r="BE2" s="48"/>
+      <c r="BF2" s="48"/>
+      <c r="BG2" s="48"/>
+      <c r="BH2" s="48"/>
+      <c r="BI2" s="48"/>
+      <c r="BJ2" s="48"/>
+      <c r="BK2" s="48"/>
+      <c r="BL2" s="48"/>
+      <c r="BM2" s="48"/>
+      <c r="BN2" s="48"/>
+    </row>
+    <row r="3" spans="1:66" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="37" t="s">
+      <c r="B3" s="32" t="s">
         <v>62</v>
       </c>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
       <c r="F3" s="9"/>
       <c r="G3" s="8"/>
       <c r="H3" s="1"/>
@@ -1297,39 +1423,39 @@
       <c r="AG3" s="1"/>
       <c r="AH3" s="1"/>
       <c r="AI3" s="1"/>
-      <c r="AJ3" s="1"/>
-      <c r="AK3" s="1"/>
-      <c r="AL3" s="1"/>
-      <c r="AM3" s="1"/>
-      <c r="AN3" s="1"/>
-      <c r="AO3" s="1"/>
-      <c r="AP3" s="1"/>
-      <c r="AQ3" s="1"/>
-      <c r="AR3" s="1"/>
-      <c r="AS3" s="1"/>
-      <c r="AT3" s="1"/>
-      <c r="AU3" s="1"/>
-      <c r="AV3" s="1"/>
-      <c r="AW3" s="1"/>
-      <c r="AX3" s="1"/>
-      <c r="AY3" s="1"/>
-      <c r="AZ3" s="1"/>
-      <c r="BA3" s="1"/>
-      <c r="BB3" s="1"/>
-      <c r="BC3" s="1"/>
-      <c r="BD3" s="1"/>
-      <c r="BE3" s="1"/>
-      <c r="BF3" s="1"/>
-      <c r="BG3" s="1"/>
-      <c r="BH3" s="1"/>
-      <c r="BI3" s="1"/>
-      <c r="BJ3" s="1"/>
-      <c r="BK3" s="1"/>
-      <c r="BL3" s="1"/>
-      <c r="BM3" s="1"/>
-      <c r="BN3" s="1"/>
-    </row>
-    <row r="4" spans="1:66" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="AJ3" s="48"/>
+      <c r="AK3" s="48"/>
+      <c r="AL3" s="48"/>
+      <c r="AM3" s="48"/>
+      <c r="AN3" s="48"/>
+      <c r="AO3" s="48"/>
+      <c r="AP3" s="48"/>
+      <c r="AQ3" s="48"/>
+      <c r="AR3" s="48"/>
+      <c r="AS3" s="48"/>
+      <c r="AT3" s="48"/>
+      <c r="AU3" s="48"/>
+      <c r="AV3" s="48"/>
+      <c r="AW3" s="48"/>
+      <c r="AX3" s="48"/>
+      <c r="AY3" s="48"/>
+      <c r="AZ3" s="48"/>
+      <c r="BA3" s="48"/>
+      <c r="BB3" s="48"/>
+      <c r="BC3" s="48"/>
+      <c r="BD3" s="48"/>
+      <c r="BE3" s="48"/>
+      <c r="BF3" s="48"/>
+      <c r="BG3" s="48"/>
+      <c r="BH3" s="48"/>
+      <c r="BI3" s="48"/>
+      <c r="BJ3" s="48"/>
+      <c r="BK3" s="48"/>
+      <c r="BL3" s="48"/>
+      <c r="BM3" s="48"/>
+      <c r="BN3" s="48"/>
+    </row>
+    <row r="4" spans="1:66" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -1345,12 +1471,12 @@
       <c r="E4">
         <v>1</v>
       </c>
-      <c r="F4" s="27">
-        <v>1</v>
-      </c>
-      <c r="G4" s="14"/>
-    </row>
-    <row r="5" spans="1:66" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="F4" s="24">
+        <v>1</v>
+      </c>
+      <c r="G4" s="30"/>
+    </row>
+    <row r="5" spans="1:66" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
@@ -1358,7 +1484,7 @@
         <v>2</v>
       </c>
       <c r="C5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D5">
         <v>2</v>
@@ -1366,535 +1492,1065 @@
       <c r="E5">
         <v>2</v>
       </c>
-      <c r="F5" s="27">
-        <v>1</v>
-      </c>
-      <c r="H5" s="14"/>
-    </row>
-    <row r="6" spans="1:66" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="F5" s="24">
+        <v>1</v>
+      </c>
+      <c r="H5" s="30"/>
+      <c r="AC5" s="43"/>
+      <c r="AD5" s="43"/>
+      <c r="AE5" s="43"/>
+      <c r="AF5" s="43"/>
+      <c r="AG5" s="43"/>
+      <c r="AH5" s="43"/>
+      <c r="AI5" s="43"/>
+    </row>
+    <row r="6" spans="1:66" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B6">
         <v>2</v>
       </c>
-      <c r="F6" s="27">
-        <v>1</v>
-      </c>
-      <c r="H6" s="14"/>
-    </row>
-    <row r="7" spans="1:66" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6" s="24">
+        <v>1</v>
+      </c>
+      <c r="H6" s="30"/>
+      <c r="I6" s="31"/>
+      <c r="AC6" s="44"/>
+      <c r="AD6" s="45" t="s">
+        <v>65</v>
+      </c>
+      <c r="AE6" s="45"/>
+      <c r="AF6" s="45"/>
+      <c r="AG6" s="45" t="s">
+        <v>68</v>
+      </c>
+      <c r="AH6" s="45"/>
+      <c r="AI6" s="45"/>
+    </row>
+    <row r="7" spans="1:66" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="8" spans="1:66" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="AC7" s="46"/>
+      <c r="AD7" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="AE7" s="45"/>
+      <c r="AF7" s="45"/>
+      <c r="AG7" s="45" t="s">
+        <v>69</v>
+      </c>
+      <c r="AH7" s="45"/>
+      <c r="AI7" s="45"/>
+    </row>
+    <row r="8" spans="1:66" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="27">
-        <v>1</v>
-      </c>
-      <c r="I8" s="15"/>
-      <c r="J8" s="15"/>
-    </row>
-    <row r="9" spans="1:66" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <v>3</v>
+      </c>
+      <c r="F8" s="24">
+        <v>1</v>
+      </c>
+      <c r="H8" s="31"/>
+      <c r="I8" s="29"/>
+      <c r="J8" s="29"/>
+      <c r="AC8" s="47"/>
+      <c r="AD8" s="45" t="s">
+        <v>66</v>
+      </c>
+      <c r="AE8" s="45"/>
+      <c r="AF8" s="45"/>
+      <c r="AG8" s="45" t="s">
+        <v>70</v>
+      </c>
+      <c r="AH8" s="45"/>
+      <c r="AI8" s="45"/>
+    </row>
+    <row r="9" spans="1:66" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="27">
-        <v>1</v>
-      </c>
-      <c r="J9" s="15"/>
-    </row>
-    <row r="10" spans="1:66" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B9">
+        <v>4</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>4</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+      <c r="F9" s="24">
+        <v>1</v>
+      </c>
+      <c r="J9" s="29"/>
+      <c r="K9" s="31"/>
+      <c r="AC9" s="46"/>
+      <c r="AD9" s="44"/>
+      <c r="AE9" s="45" t="s">
+        <v>67</v>
+      </c>
+      <c r="AF9" s="45"/>
+      <c r="AG9" s="45" t="s">
+        <v>71</v>
+      </c>
+      <c r="AH9" s="45"/>
+      <c r="AI9" s="45"/>
+    </row>
+    <row r="10" spans="1:66" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F10" s="27">
-        <v>1</v>
-      </c>
-      <c r="K10" s="15"/>
-    </row>
-    <row r="11" spans="1:66" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B10">
+        <v>5</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>5</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10" s="24">
+        <v>1</v>
+      </c>
+      <c r="K10" s="29"/>
+      <c r="AC10" s="19"/>
+      <c r="AD10" s="19"/>
+      <c r="AE10" s="19"/>
+      <c r="AF10" s="19"/>
+      <c r="AG10" s="19"/>
+      <c r="AH10" s="19"/>
+      <c r="AI10" s="19"/>
+    </row>
+    <row r="11" spans="1:66" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F11" s="27">
-        <v>1</v>
-      </c>
-      <c r="L11" s="15"/>
-      <c r="M11" s="15"/>
-    </row>
-    <row r="12" spans="1:66" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B11">
+        <v>6</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11">
+        <v>6</v>
+      </c>
+      <c r="E11">
+        <v>2</v>
+      </c>
+      <c r="F11" s="24">
+        <v>1</v>
+      </c>
+      <c r="L11" s="29"/>
+      <c r="M11" s="29"/>
+    </row>
+    <row r="12" spans="1:66" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="12" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="13" spans="1:66" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:66" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F13" s="27">
-        <v>1</v>
-      </c>
-      <c r="K13" s="16"/>
-    </row>
-    <row r="14" spans="1:66" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B13">
+        <v>5</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>5</v>
+      </c>
+      <c r="E13">
+        <v>2</v>
+      </c>
+      <c r="F13" s="24">
+        <v>1</v>
+      </c>
+      <c r="K13" s="39"/>
+      <c r="L13" s="31"/>
+    </row>
+    <row r="14" spans="1:66" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>14</v>
       </c>
+      <c r="B14">
+        <v>6</v>
+      </c>
+      <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="D14">
+        <v>6</v>
+      </c>
+      <c r="E14">
+        <v>3</v>
+      </c>
       <c r="F14" t="s">
         <v>61</v>
       </c>
-      <c r="L14" s="16"/>
-      <c r="M14" s="16"/>
-    </row>
-    <row r="15" spans="1:66" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="L14" s="39"/>
+      <c r="M14" s="39"/>
+      <c r="N14" s="31"/>
+    </row>
+    <row r="15" spans="1:66" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>15</v>
       </c>
+      <c r="B15">
+        <v>7</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>7</v>
+      </c>
+      <c r="E15">
+        <v>2</v>
+      </c>
       <c r="F15" t="s">
         <v>61</v>
       </c>
-      <c r="M15" s="16"/>
-    </row>
-    <row r="16" spans="1:66" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="M15" s="39"/>
+      <c r="N15" s="31"/>
+    </row>
+    <row r="16" spans="1:66" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>16</v>
       </c>
+      <c r="B16">
+        <v>7</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="D16">
+        <v>7</v>
+      </c>
+      <c r="E16">
+        <v>3</v>
+      </c>
       <c r="F16" t="s">
         <v>61</v>
       </c>
-      <c r="M16" s="16"/>
-      <c r="N16" s="16"/>
-    </row>
-    <row r="17" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="M16" s="39"/>
+      <c r="N16" s="39"/>
+      <c r="O16" s="31"/>
+    </row>
+    <row r="17" spans="1:20" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="13" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:20" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F18" s="27">
-        <v>1</v>
-      </c>
-      <c r="L18" s="17"/>
-    </row>
-    <row r="19" spans="1:20" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B18">
+        <v>6</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>6</v>
+      </c>
+      <c r="E18">
+        <v>2</v>
+      </c>
+      <c r="F18" s="24">
+        <v>1</v>
+      </c>
+      <c r="L18" s="40"/>
+      <c r="M18" s="31"/>
+    </row>
+    <row r="19" spans="1:20" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F19" s="27">
-        <v>1</v>
-      </c>
-      <c r="M19" s="17"/>
-    </row>
-    <row r="20" spans="1:20" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B19">
+        <v>7</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>7</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19" s="24">
+        <v>1</v>
+      </c>
+      <c r="M19" s="40"/>
+    </row>
+    <row r="20" spans="1:20" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F20" s="27">
-        <v>1</v>
-      </c>
-      <c r="M20" s="17"/>
-    </row>
-    <row r="21" spans="1:20" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B20">
+        <v>7</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <v>7</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20" s="24">
+        <v>1</v>
+      </c>
+      <c r="M20" s="40"/>
+    </row>
+    <row r="21" spans="1:20" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F21" s="27">
-        <v>1</v>
-      </c>
-      <c r="M21" s="17"/>
-      <c r="N21" s="17"/>
-    </row>
-    <row r="22" spans="1:20" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B21">
+        <v>7</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
+      </c>
+      <c r="D21">
+        <v>7</v>
+      </c>
+      <c r="E21">
+        <v>3</v>
+      </c>
+      <c r="F21" s="24">
+        <v>1</v>
+      </c>
+      <c r="M21" s="40"/>
+      <c r="N21" s="40"/>
+      <c r="O21" s="31"/>
+    </row>
+    <row r="22" spans="1:20" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="F22" s="27">
-        <v>1</v>
-      </c>
-      <c r="N22" s="17"/>
-      <c r="O22" s="17"/>
-      <c r="P22" s="17"/>
-    </row>
-    <row r="23" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B22">
+        <v>8</v>
+      </c>
+      <c r="C22">
+        <v>3</v>
+      </c>
+      <c r="D22">
+        <v>8</v>
+      </c>
+      <c r="E22">
+        <v>4</v>
+      </c>
+      <c r="F22" s="24">
+        <v>1</v>
+      </c>
+      <c r="N22" s="40"/>
+      <c r="O22" s="40"/>
+      <c r="P22" s="40"/>
+      <c r="Q22" s="31"/>
+    </row>
+    <row r="23" spans="1:20" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="13" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="24" spans="1:20" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:20" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F24" s="27">
-        <v>1</v>
-      </c>
-      <c r="P24" s="18"/>
-      <c r="Q24" s="18"/>
-    </row>
-    <row r="25" spans="1:20" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B24">
+        <v>10</v>
+      </c>
+      <c r="C24">
+        <v>2</v>
+      </c>
+      <c r="D24">
+        <v>10</v>
+      </c>
+      <c r="E24">
+        <v>4</v>
+      </c>
+      <c r="F24" s="24">
+        <v>1</v>
+      </c>
+      <c r="P24" s="41"/>
+      <c r="Q24" s="41"/>
+      <c r="R24" s="31"/>
+      <c r="S24" s="31"/>
+    </row>
+    <row r="25" spans="1:20" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F25" s="27">
-        <v>1</v>
-      </c>
-      <c r="R25" s="18"/>
-    </row>
-    <row r="26" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B25">
+        <v>12</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <v>13</v>
+      </c>
+      <c r="E25">
+        <v>2</v>
+      </c>
+      <c r="F25" s="24">
+        <v>1</v>
+      </c>
+      <c r="R25" s="15"/>
+      <c r="S25" s="31"/>
+      <c r="T25" s="31"/>
+    </row>
+    <row r="26" spans="1:20" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="13" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="27" spans="1:20" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A27" s="28" t="s">
+    <row r="27" spans="1:20" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A27" s="25" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:20" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:20" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F28" s="27">
+      <c r="B28">
+        <v>8</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="F28" s="24">
         <v>0</v>
       </c>
-      <c r="N28" s="19"/>
-    </row>
-    <row r="29" spans="1:20" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="N28" s="16"/>
+    </row>
+    <row r="29" spans="1:20" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="F29" s="27">
+      <c r="B29">
+        <v>9</v>
+      </c>
+      <c r="C29">
+        <v>2</v>
+      </c>
+      <c r="F29" s="24">
         <v>0</v>
       </c>
-      <c r="O29" s="19"/>
-      <c r="P29" s="19"/>
-    </row>
-    <row r="30" spans="1:20" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="O29" s="16"/>
+      <c r="P29" s="16"/>
+    </row>
+    <row r="30" spans="1:20" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F30" s="27">
+      <c r="B30">
+        <v>10</v>
+      </c>
+      <c r="C30">
+        <v>3</v>
+      </c>
+      <c r="F30" s="24">
         <v>0</v>
       </c>
-      <c r="P30" s="19"/>
-      <c r="Q30" s="19"/>
-      <c r="R30" s="19"/>
-    </row>
-    <row r="31" spans="1:20" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="P30" s="16"/>
+      <c r="Q30" s="16"/>
+      <c r="R30" s="16"/>
+    </row>
+    <row r="31" spans="1:20" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F31" s="27">
+      <c r="B31">
+        <v>11</v>
+      </c>
+      <c r="C31">
+        <v>4</v>
+      </c>
+      <c r="F31" s="24">
         <v>0</v>
       </c>
-      <c r="Q31" s="19"/>
-      <c r="R31" s="19"/>
-      <c r="S31" s="19"/>
-      <c r="T31" s="19"/>
-    </row>
-    <row r="32" spans="1:20" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="Q31" s="16"/>
+      <c r="R31" s="16"/>
+      <c r="S31" s="16"/>
+      <c r="T31" s="16"/>
+    </row>
+    <row r="32" spans="1:20" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F32" s="27">
+      <c r="B32">
+        <v>13</v>
+      </c>
+      <c r="C32">
+        <v>2</v>
+      </c>
+      <c r="F32" s="24">
         <v>0</v>
       </c>
-      <c r="S32" s="19"/>
-      <c r="T32" s="19"/>
-    </row>
-    <row r="33" spans="1:29" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A33" s="29" t="s">
+      <c r="S32" s="16"/>
+      <c r="T32" s="16"/>
+    </row>
+    <row r="33" spans="1:29" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A33" s="26" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="1:29" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:29" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F34" s="27">
+      <c r="B34">
+        <v>9</v>
+      </c>
+      <c r="C34">
+        <v>1</v>
+      </c>
+      <c r="F34" s="24">
         <v>0</v>
       </c>
-      <c r="O34" s="19"/>
-    </row>
-    <row r="35" spans="1:29" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="O34" s="16"/>
+    </row>
+    <row r="35" spans="1:29" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F35" s="27">
+      <c r="B35">
+        <v>10</v>
+      </c>
+      <c r="C35">
+        <v>2</v>
+      </c>
+      <c r="F35" s="24">
         <v>0</v>
       </c>
-      <c r="P35" s="19"/>
-      <c r="Q35" s="19"/>
-    </row>
-    <row r="36" spans="1:29" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="P35" s="16"/>
+      <c r="Q35" s="16"/>
+    </row>
+    <row r="36" spans="1:29" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F36" s="27">
+      <c r="B36">
+        <v>11</v>
+      </c>
+      <c r="C36">
+        <v>3</v>
+      </c>
+      <c r="F36" s="24">
         <v>0</v>
       </c>
-      <c r="Q36" s="19"/>
-      <c r="R36" s="19"/>
-      <c r="S36" s="19"/>
-    </row>
-    <row r="37" spans="1:29" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="Q36" s="16"/>
+      <c r="R36" s="16"/>
+      <c r="S36" s="16"/>
+    </row>
+    <row r="37" spans="1:29" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="F37" s="27">
+      <c r="B37">
+        <v>13</v>
+      </c>
+      <c r="C37">
+        <v>2</v>
+      </c>
+      <c r="F37" s="24">
         <v>0</v>
       </c>
-      <c r="S37" s="19"/>
-      <c r="T37" s="19"/>
-    </row>
-    <row r="38" spans="1:29" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="S37" s="16"/>
+      <c r="T37" s="16"/>
+    </row>
+    <row r="38" spans="1:29" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="F38" s="27">
+      <c r="B38">
+        <v>12</v>
+      </c>
+      <c r="C38">
+        <v>4</v>
+      </c>
+      <c r="F38" s="24">
         <v>0</v>
       </c>
-      <c r="R38" s="19"/>
-      <c r="S38" s="19"/>
-      <c r="T38" s="19"/>
-      <c r="U38" s="19"/>
-    </row>
-    <row r="39" spans="1:29" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="R38" s="16"/>
+      <c r="S38" s="16"/>
+      <c r="T38" s="16"/>
+      <c r="U38" s="16"/>
+    </row>
+    <row r="39" spans="1:29" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="13" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="40" spans="1:29" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:29" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="F40" s="27">
+      <c r="B40">
+        <v>14</v>
+      </c>
+      <c r="C40">
+        <v>3</v>
+      </c>
+      <c r="F40" s="24">
         <v>0</v>
       </c>
-      <c r="T40" s="20"/>
-      <c r="U40" s="20"/>
-      <c r="V40" s="20"/>
-    </row>
-    <row r="41" spans="1:29" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="T40" s="17"/>
+      <c r="U40" s="17"/>
+      <c r="V40" s="17"/>
+    </row>
+    <row r="41" spans="1:29" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="F41" s="27">
+      <c r="B41">
+        <v>16</v>
+      </c>
+      <c r="C41">
+        <v>1</v>
+      </c>
+      <c r="F41" s="24">
         <v>0</v>
       </c>
-      <c r="V41" s="20"/>
-    </row>
-    <row r="42" spans="1:29" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="V41" s="17"/>
+    </row>
+    <row r="42" spans="1:29" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="F42" s="27">
+      <c r="B42">
+        <v>16</v>
+      </c>
+      <c r="C42">
+        <v>2</v>
+      </c>
+      <c r="F42" s="24">
         <v>0</v>
       </c>
-      <c r="V42" s="20"/>
-      <c r="W42" s="20"/>
-    </row>
-    <row r="43" spans="1:29" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="V42" s="17"/>
+      <c r="W42" s="17"/>
+    </row>
+    <row r="43" spans="1:29" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="F43" s="27">
+      <c r="B43">
+        <v>18</v>
+      </c>
+      <c r="C43">
+        <v>1</v>
+      </c>
+      <c r="F43" s="24">
         <v>0</v>
       </c>
-      <c r="X43" s="20"/>
-    </row>
-    <row r="44" spans="1:29" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="X43" s="17"/>
+    </row>
+    <row r="44" spans="1:29" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="N44" s="22"/>
-      <c r="O44" s="22"/>
-      <c r="P44" s="22"/>
-      <c r="Q44" s="22"/>
-      <c r="R44" s="22"/>
-      <c r="S44" s="22"/>
-      <c r="T44" s="22"/>
-      <c r="U44" s="22"/>
-      <c r="V44" s="22"/>
-      <c r="W44" s="22"/>
-      <c r="X44" s="22"/>
-      <c r="Y44" s="22"/>
-      <c r="Z44" s="22"/>
-    </row>
-    <row r="45" spans="1:29" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="N44" s="19"/>
+      <c r="O44" s="19"/>
+      <c r="P44" s="19"/>
+      <c r="Q44" s="19"/>
+      <c r="R44" s="19"/>
+      <c r="S44" s="19"/>
+      <c r="T44" s="19"/>
+      <c r="U44" s="19"/>
+      <c r="V44" s="19"/>
+      <c r="W44" s="19"/>
+      <c r="X44" s="19"/>
+      <c r="Y44" s="19"/>
+      <c r="Z44" s="19"/>
+    </row>
+    <row r="45" spans="1:29" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="F45" s="27">
+      <c r="B45">
+        <v>13</v>
+      </c>
+      <c r="C45">
+        <v>7</v>
+      </c>
+      <c r="F45" s="24">
         <v>0</v>
       </c>
-      <c r="N45" s="22"/>
-      <c r="O45" s="22"/>
-      <c r="P45" s="23"/>
-      <c r="Q45" s="23"/>
-      <c r="R45" s="23"/>
-      <c r="S45" s="24"/>
-      <c r="T45" s="24"/>
-      <c r="U45" s="24"/>
-      <c r="V45" s="24"/>
-      <c r="W45" s="24"/>
-      <c r="X45" s="24"/>
-      <c r="Y45" s="24"/>
-      <c r="Z45" s="22"/>
-    </row>
-    <row r="46" spans="1:29" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="N45" s="19"/>
+      <c r="O45" s="19"/>
+      <c r="P45" s="20"/>
+      <c r="Q45" s="20"/>
+      <c r="R45" s="20"/>
+      <c r="S45" s="21"/>
+      <c r="T45" s="21"/>
+      <c r="U45" s="21"/>
+      <c r="V45" s="21"/>
+      <c r="W45" s="21"/>
+      <c r="X45" s="21"/>
+      <c r="Y45" s="21"/>
+      <c r="Z45" s="19"/>
+    </row>
+    <row r="46" spans="1:29" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="F46" s="27">
+      <c r="B46">
+        <v>17</v>
+      </c>
+      <c r="C46">
+        <v>5</v>
+      </c>
+      <c r="F46" s="24">
         <v>0</v>
       </c>
-      <c r="N46" s="22"/>
-      <c r="O46" s="22"/>
-      <c r="P46" s="22"/>
-      <c r="Q46" s="22"/>
-      <c r="R46" s="22"/>
-      <c r="S46" s="22"/>
-      <c r="T46" s="22"/>
-      <c r="U46" s="22"/>
-      <c r="V46" s="22"/>
-      <c r="W46" s="21"/>
-      <c r="X46" s="21"/>
-      <c r="Y46" s="21"/>
-      <c r="Z46" s="21"/>
-      <c r="AA46" s="21"/>
-    </row>
-    <row r="47" spans="1:29" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="N46" s="19"/>
+      <c r="O46" s="19"/>
+      <c r="P46" s="19"/>
+      <c r="Q46" s="19"/>
+      <c r="R46" s="19"/>
+      <c r="S46" s="19"/>
+      <c r="T46" s="19"/>
+      <c r="U46" s="19"/>
+      <c r="V46" s="19"/>
+      <c r="W46" s="18"/>
+      <c r="X46" s="18"/>
+      <c r="Y46" s="18"/>
+      <c r="Z46" s="18"/>
+      <c r="AA46" s="18"/>
+    </row>
+    <row r="47" spans="1:29" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="F47" s="27">
+      <c r="B47">
+        <v>20</v>
+      </c>
+      <c r="C47">
+        <v>3</v>
+      </c>
+      <c r="F47" s="24">
         <v>0</v>
       </c>
-      <c r="N47" s="22"/>
-      <c r="O47" s="22"/>
-      <c r="P47" s="22"/>
-      <c r="Q47" s="22"/>
-      <c r="R47" s="22"/>
-      <c r="S47" s="22"/>
-      <c r="T47" s="22"/>
-      <c r="U47" s="22"/>
-      <c r="V47" s="22"/>
-      <c r="W47" s="22"/>
-      <c r="X47" s="22"/>
-      <c r="Y47" s="22"/>
-      <c r="Z47" s="21"/>
-      <c r="AA47" s="21"/>
-      <c r="AB47" s="21"/>
-    </row>
-    <row r="48" spans="1:29" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="N47" s="19"/>
+      <c r="O47" s="19"/>
+      <c r="P47" s="19"/>
+      <c r="Q47" s="19"/>
+      <c r="R47" s="19"/>
+      <c r="S47" s="19"/>
+      <c r="T47" s="19"/>
+      <c r="U47" s="19"/>
+      <c r="V47" s="19"/>
+      <c r="W47" s="19"/>
+      <c r="X47" s="19"/>
+      <c r="Y47" s="19"/>
+      <c r="Z47" s="18"/>
+      <c r="AA47" s="18"/>
+      <c r="AB47" s="18"/>
+    </row>
+    <row r="48" spans="1:29" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="F48" s="27">
+      <c r="B48">
+        <v>23</v>
+      </c>
+      <c r="C48">
+        <v>1</v>
+      </c>
+      <c r="F48" s="24">
         <v>0</v>
       </c>
-      <c r="AC48" s="21"/>
-    </row>
-    <row r="49" spans="1:35" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AC48" s="18"/>
+    </row>
+    <row r="49" spans="1:35" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="13" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="50" spans="1:35" ht="17.399999999999999" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="50" spans="1:35" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="7" t="s">
         <v>44</v>
       </c>
+      <c r="B50">
+        <v>9</v>
+      </c>
+      <c r="C50">
+        <v>7</v>
+      </c>
+      <c r="D50">
+        <v>9</v>
+      </c>
+      <c r="E50">
+        <v>7</v>
+      </c>
       <c r="F50" t="s">
         <v>61</v>
       </c>
-      <c r="AD50" s="25"/>
-      <c r="AE50" s="25"/>
-    </row>
-    <row r="51" spans="1:35" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="O50" s="42"/>
+      <c r="P50" s="42"/>
+      <c r="Q50" s="42"/>
+      <c r="R50" s="42"/>
+      <c r="S50" s="42"/>
+      <c r="T50" s="42"/>
+      <c r="U50" s="42"/>
+      <c r="V50" s="19"/>
+      <c r="W50" s="19"/>
+      <c r="X50" s="19"/>
+      <c r="Y50" s="19"/>
+      <c r="Z50" s="19"/>
+      <c r="AA50" s="28"/>
+      <c r="AB50" s="28"/>
+      <c r="AC50" s="28"/>
+      <c r="AD50" s="22"/>
+      <c r="AE50" s="22"/>
+    </row>
+    <row r="51" spans="1:35" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
         <v>45</v>
       </c>
+      <c r="B51">
+        <v>13</v>
+      </c>
+      <c r="C51">
+        <v>3</v>
+      </c>
+      <c r="D51">
+        <v>13</v>
+      </c>
+      <c r="E51">
+        <v>3</v>
+      </c>
       <c r="F51" t="s">
         <v>61</v>
       </c>
-      <c r="AE51" s="25"/>
-      <c r="AF51" s="25"/>
-    </row>
-    <row r="52" spans="1:35" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="S51" s="42"/>
+      <c r="T51" s="42"/>
+      <c r="U51" s="42"/>
+      <c r="AA51" s="19"/>
+      <c r="AB51" s="19"/>
+      <c r="AC51" s="19"/>
+      <c r="AD51" s="28"/>
+      <c r="AE51" s="22"/>
+      <c r="AF51" s="22"/>
+    </row>
+    <row r="52" spans="1:35" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
         <v>46</v>
       </c>
+      <c r="B52">
+        <v>15</v>
+      </c>
+      <c r="C52">
+        <v>1</v>
+      </c>
+      <c r="D52">
+        <v>15</v>
+      </c>
+      <c r="E52">
+        <v>1</v>
+      </c>
       <c r="F52" t="s">
         <v>61</v>
       </c>
-      <c r="AD52" s="25"/>
-      <c r="AE52" s="25"/>
-      <c r="AF52" s="25"/>
-    </row>
-    <row r="53" spans="1:35" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="U52" s="42"/>
+      <c r="AD52" s="19"/>
+      <c r="AE52" s="22"/>
+      <c r="AF52" s="22"/>
+    </row>
+    <row r="53" spans="1:35" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
         <v>47</v>
       </c>
+      <c r="B53">
+        <v>10</v>
+      </c>
+      <c r="C53">
+        <v>6</v>
+      </c>
+      <c r="D53">
+        <v>10</v>
+      </c>
+      <c r="E53">
+        <v>6</v>
+      </c>
       <c r="F53" t="s">
         <v>61</v>
       </c>
-      <c r="AG53" s="25"/>
-    </row>
-    <row r="54" spans="1:35" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="P53" s="42"/>
+      <c r="Q53" s="42"/>
+      <c r="R53" s="42"/>
+      <c r="S53" s="42"/>
+      <c r="T53" s="42"/>
+      <c r="U53" s="42"/>
+      <c r="V53" s="19"/>
+      <c r="W53" s="19"/>
+      <c r="X53" s="19"/>
+      <c r="Y53" s="19"/>
+      <c r="Z53" s="19"/>
+      <c r="AA53" s="28"/>
+      <c r="AB53" s="28"/>
+      <c r="AC53" s="28"/>
+      <c r="AD53" s="28"/>
+      <c r="AE53" s="28"/>
+      <c r="AF53" s="28"/>
+      <c r="AG53" s="28"/>
+    </row>
+    <row r="54" spans="1:35" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
         <v>48</v>
       </c>
+      <c r="B54">
+        <v>15</v>
+      </c>
+      <c r="C54">
+        <v>1</v>
+      </c>
+      <c r="D54">
+        <v>15</v>
+      </c>
+      <c r="E54">
+        <v>1</v>
+      </c>
       <c r="F54" t="s">
         <v>61</v>
       </c>
-      <c r="AG54" s="25"/>
-    </row>
-    <row r="55" spans="1:35" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="U54" s="42"/>
+      <c r="X54" s="19"/>
+      <c r="Y54" s="19"/>
+      <c r="Z54" s="19"/>
+      <c r="AA54" s="19"/>
+      <c r="AB54" s="19"/>
+      <c r="AC54" s="19"/>
+      <c r="AD54" s="19"/>
+      <c r="AE54" s="28"/>
+      <c r="AF54" s="28"/>
+      <c r="AG54" s="22"/>
+    </row>
+    <row r="55" spans="1:35" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="5" t="s">
         <v>49</v>
       </c>
+      <c r="B55">
+        <v>15</v>
+      </c>
+      <c r="C55">
+        <v>1</v>
+      </c>
+      <c r="D55">
+        <v>15</v>
+      </c>
+      <c r="E55">
+        <v>2</v>
+      </c>
       <c r="F55" t="s">
         <v>61</v>
       </c>
-      <c r="AD55" s="25"/>
-      <c r="AE55" s="25"/>
-      <c r="AF55" s="25"/>
-      <c r="AG55" s="25"/>
-      <c r="AH55" s="25"/>
-    </row>
-    <row r="56" spans="1:35" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="U55" s="42"/>
+      <c r="V55" s="31"/>
+      <c r="AD55" s="19"/>
+      <c r="AE55" s="19"/>
+      <c r="AF55" s="19"/>
+      <c r="AG55" s="22"/>
+      <c r="AH55" s="22"/>
+    </row>
+    <row r="56" spans="1:35" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="13" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="57" spans="1:35" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:35" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="F57" s="27">
-        <v>0</v>
-      </c>
-      <c r="AH57" s="26"/>
-      <c r="AI57" s="26"/>
-    </row>
-    <row r="58" spans="1:35" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B57">
+        <v>15</v>
+      </c>
+      <c r="C57">
+        <v>2</v>
+      </c>
+      <c r="D57">
+        <v>16</v>
+      </c>
+      <c r="E57">
+        <v>1</v>
+      </c>
+      <c r="F57" s="24">
+        <v>0.5</v>
+      </c>
+      <c r="U57" s="14"/>
+      <c r="V57" s="31"/>
+      <c r="AH57" s="23"/>
+      <c r="AI57" s="23"/>
+    </row>
+    <row r="58" spans="1:35" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="F58" s="27">
-        <v>0</v>
-      </c>
-      <c r="AI58" s="26"/>
-    </row>
+      <c r="B58">
+        <v>16</v>
+      </c>
+      <c r="C58">
+        <v>1</v>
+      </c>
+      <c r="D58">
+        <v>17</v>
+      </c>
+      <c r="E58">
+        <v>1</v>
+      </c>
+      <c r="F58" s="24">
+        <v>0.5</v>
+      </c>
+      <c r="V58" s="14"/>
+      <c r="W58" s="31"/>
+      <c r="AI58" s="23"/>
+    </row>
+    <row r="59" spans="1:35" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="16">
+    <mergeCell ref="AG6:AI6"/>
+    <mergeCell ref="AG7:AI7"/>
+    <mergeCell ref="AG8:AI8"/>
+    <mergeCell ref="AG9:AI9"/>
+    <mergeCell ref="AD6:AF6"/>
+    <mergeCell ref="AD8:AF8"/>
+    <mergeCell ref="AD7:AF7"/>
+    <mergeCell ref="AE9:AF9"/>
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="G1:AI1"/>
     <mergeCell ref="A1:A2"/>
@@ -1919,6 +2575,6 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Periods are charted from 1 to 60 starting from cell H4 to cell BO4 " sqref="G1" xr:uid="{5A1C689C-859F-4C11-8B55-50D065957DF7}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="44" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Everything is ready for submission
</commit_message>
<xml_diff>
--- a/Gantt chart.xlsx
+++ b/Gantt chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pranj\software-tech-ass\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F553B48-5D24-4F2F-A95E-42EFA6E0D0CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C900504-1309-4D1F-9259-A166D908B309}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,6 @@
     <definedName name="TitleRegion..BO60">#REF!</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -45,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="73">
   <si>
     <t>ACTIVITY</t>
   </si>
@@ -125,18 +124,9 @@
     <t>Set up project structure and environment</t>
   </si>
   <si>
-    <t>Implement data loading and preprocessing</t>
-  </si>
-  <si>
     <t>Develop user interface components</t>
   </si>
   <si>
-    <t>Implement analysis algorithms</t>
-  </si>
-  <si>
-    <t>Integrate UI and analysis components</t>
-  </si>
-  <si>
     <t>Perform Unit Testing</t>
   </si>
   <si>
@@ -261,6 +251,18 @@
   </si>
   <si>
     <t>lining after color</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data Analysis and insights </t>
+  </si>
+  <si>
+    <t>Implement data analysis algorithms with UI</t>
+  </si>
+  <si>
+    <t>Integrate 5 types of insight tools</t>
+  </si>
+  <si>
+    <t>Data visualization</t>
   </si>
 </sst>
 </file>
@@ -560,7 +562,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -666,6 +668,43 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
@@ -724,7 +763,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -821,6 +860,33 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="15" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="3" xfId="15" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="3" xfId="15" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="3" xfId="15" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="3" xfId="15" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="8" xfId="15" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="28" borderId="8" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="0" borderId="0" xfId="3" applyBorder="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="10" applyBorder="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -842,35 +908,14 @@
     <xf numFmtId="0" fontId="6" fillId="17" borderId="5" xfId="10" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="3" xfId="15" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="3" xfId="15" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="3" xfId="15" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="25" borderId="3" xfId="15" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="8" xfId="15" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="26" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="26" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="15" fillId="26" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="28" borderId="8" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="0" borderId="0" xfId="3" applyBorder="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="15" fillId="26" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -1158,73 +1203,73 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BN59"/>
+  <dimension ref="A1:BN60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="72" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AO44" sqref="AO44"/>
+    <sheetView tabSelected="1" zoomScale="30" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AJ59" sqref="A1:AJ59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="53.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="66" width="4.75" customWidth="1"/>
+    <col min="1" max="1" width="53.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="66" width="4.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:66" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
+    <row r="1" spans="1:66" x14ac:dyDescent="0.3">
+      <c r="A1" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="36" t="s">
+      <c r="B1" s="45" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="36" t="s">
+      <c r="D1" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="36" t="s">
+      <c r="E1" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="38" t="s">
+      <c r="F1" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="33" t="s">
-        <v>62</v>
-      </c>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="33"/>
-      <c r="L1" s="33"/>
-      <c r="M1" s="33"/>
-      <c r="N1" s="33"/>
-      <c r="O1" s="33"/>
-      <c r="P1" s="33"/>
-      <c r="Q1" s="33"/>
-      <c r="R1" s="33"/>
-      <c r="S1" s="33"/>
-      <c r="T1" s="33"/>
-      <c r="U1" s="33"/>
-      <c r="V1" s="33"/>
-      <c r="W1" s="33"/>
-      <c r="X1" s="33"/>
-      <c r="Y1" s="33"/>
-      <c r="Z1" s="33"/>
-      <c r="AA1" s="33"/>
-      <c r="AB1" s="33"/>
-      <c r="AC1" s="33"/>
-      <c r="AD1" s="33"/>
-      <c r="AE1" s="33"/>
-      <c r="AF1" s="33"/>
-      <c r="AG1" s="33"/>
-      <c r="AH1" s="33"/>
-      <c r="AI1" s="33"/>
+      <c r="G1" s="42" t="s">
+        <v>59</v>
+      </c>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
+      <c r="K1" s="42"/>
+      <c r="L1" s="42"/>
+      <c r="M1" s="42"/>
+      <c r="N1" s="42"/>
+      <c r="O1" s="42"/>
+      <c r="P1" s="42"/>
+      <c r="Q1" s="42"/>
+      <c r="R1" s="42"/>
+      <c r="S1" s="42"/>
+      <c r="T1" s="42"/>
+      <c r="U1" s="42"/>
+      <c r="V1" s="42"/>
+      <c r="W1" s="42"/>
+      <c r="X1" s="42"/>
+      <c r="Y1" s="42"/>
+      <c r="Z1" s="42"/>
+      <c r="AA1" s="42"/>
+      <c r="AB1" s="42"/>
+      <c r="AC1" s="42"/>
+      <c r="AD1" s="42"/>
+      <c r="AE1" s="42"/>
+      <c r="AF1" s="42"/>
+      <c r="AG1" s="42"/>
+      <c r="AH1" s="42"/>
+      <c r="AI1" s="42"/>
       <c r="AJ1" s="2"/>
       <c r="AK1" s="2"/>
       <c r="AL1" s="2"/>
@@ -1257,13 +1302,13 @@
       <c r="BM1" s="2"/>
       <c r="BN1" s="2"/>
     </row>
-    <row r="2" spans="1:66" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="35"/>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
+    <row r="2" spans="1:66" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="44"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
       <c r="G2" s="27">
         <v>1</v>
       </c>
@@ -1351,48 +1396,48 @@
       <c r="AI2" s="27">
         <v>29</v>
       </c>
-      <c r="AJ2" s="48"/>
-      <c r="AK2" s="48"/>
-      <c r="AL2" s="48"/>
-      <c r="AM2" s="48"/>
-      <c r="AN2" s="48"/>
-      <c r="AO2" s="48"/>
-      <c r="AP2" s="48"/>
-      <c r="AQ2" s="48"/>
-      <c r="AR2" s="48"/>
-      <c r="AS2" s="48"/>
-      <c r="AT2" s="48"/>
-      <c r="AU2" s="48"/>
-      <c r="AV2" s="48"/>
-      <c r="AW2" s="48"/>
-      <c r="AX2" s="48"/>
-      <c r="AY2" s="48"/>
-      <c r="AZ2" s="48"/>
-      <c r="BA2" s="48"/>
-      <c r="BB2" s="48"/>
-      <c r="BC2" s="48"/>
-      <c r="BD2" s="48"/>
-      <c r="BE2" s="48"/>
-      <c r="BF2" s="48"/>
-      <c r="BG2" s="48"/>
-      <c r="BH2" s="48"/>
-      <c r="BI2" s="48"/>
-      <c r="BJ2" s="48"/>
-      <c r="BK2" s="48"/>
-      <c r="BL2" s="48"/>
-      <c r="BM2" s="48"/>
-      <c r="BN2" s="48"/>
-    </row>
-    <row r="3" spans="1:66" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AJ2" s="40"/>
+      <c r="AK2" s="40"/>
+      <c r="AL2" s="40"/>
+      <c r="AM2" s="40"/>
+      <c r="AN2" s="40"/>
+      <c r="AO2" s="40"/>
+      <c r="AP2" s="40"/>
+      <c r="AQ2" s="40"/>
+      <c r="AR2" s="40"/>
+      <c r="AS2" s="40"/>
+      <c r="AT2" s="40"/>
+      <c r="AU2" s="40"/>
+      <c r="AV2" s="40"/>
+      <c r="AW2" s="40"/>
+      <c r="AX2" s="40"/>
+      <c r="AY2" s="40"/>
+      <c r="AZ2" s="40"/>
+      <c r="BA2" s="40"/>
+      <c r="BB2" s="40"/>
+      <c r="BC2" s="40"/>
+      <c r="BD2" s="40"/>
+      <c r="BE2" s="40"/>
+      <c r="BF2" s="40"/>
+      <c r="BG2" s="40"/>
+      <c r="BH2" s="40"/>
+      <c r="BI2" s="40"/>
+      <c r="BJ2" s="40"/>
+      <c r="BK2" s="40"/>
+      <c r="BL2" s="40"/>
+      <c r="BM2" s="40"/>
+      <c r="BN2" s="40"/>
+    </row>
+    <row r="3" spans="1:66" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="B3" s="32" t="s">
-        <v>62</v>
-      </c>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
+        <v>49</v>
+      </c>
+      <c r="B3" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
       <c r="F3" s="9"/>
       <c r="G3" s="8"/>
       <c r="H3" s="1"/>
@@ -1423,39 +1468,39 @@
       <c r="AG3" s="1"/>
       <c r="AH3" s="1"/>
       <c r="AI3" s="1"/>
-      <c r="AJ3" s="48"/>
-      <c r="AK3" s="48"/>
-      <c r="AL3" s="48"/>
-      <c r="AM3" s="48"/>
-      <c r="AN3" s="48"/>
-      <c r="AO3" s="48"/>
-      <c r="AP3" s="48"/>
-      <c r="AQ3" s="48"/>
-      <c r="AR3" s="48"/>
-      <c r="AS3" s="48"/>
-      <c r="AT3" s="48"/>
-      <c r="AU3" s="48"/>
-      <c r="AV3" s="48"/>
-      <c r="AW3" s="48"/>
-      <c r="AX3" s="48"/>
-      <c r="AY3" s="48"/>
-      <c r="AZ3" s="48"/>
-      <c r="BA3" s="48"/>
-      <c r="BB3" s="48"/>
-      <c r="BC3" s="48"/>
-      <c r="BD3" s="48"/>
-      <c r="BE3" s="48"/>
-      <c r="BF3" s="48"/>
-      <c r="BG3" s="48"/>
-      <c r="BH3" s="48"/>
-      <c r="BI3" s="48"/>
-      <c r="BJ3" s="48"/>
-      <c r="BK3" s="48"/>
-      <c r="BL3" s="48"/>
-      <c r="BM3" s="48"/>
-      <c r="BN3" s="48"/>
-    </row>
-    <row r="4" spans="1:66" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AJ3" s="40"/>
+      <c r="AK3" s="40"/>
+      <c r="AL3" s="40"/>
+      <c r="AM3" s="40"/>
+      <c r="AN3" s="40"/>
+      <c r="AO3" s="40"/>
+      <c r="AP3" s="40"/>
+      <c r="AQ3" s="40"/>
+      <c r="AR3" s="40"/>
+      <c r="AS3" s="40"/>
+      <c r="AT3" s="40"/>
+      <c r="AU3" s="40"/>
+      <c r="AV3" s="40"/>
+      <c r="AW3" s="40"/>
+      <c r="AX3" s="40"/>
+      <c r="AY3" s="40"/>
+      <c r="AZ3" s="40"/>
+      <c r="BA3" s="40"/>
+      <c r="BB3" s="40"/>
+      <c r="BC3" s="40"/>
+      <c r="BD3" s="40"/>
+      <c r="BE3" s="40"/>
+      <c r="BF3" s="40"/>
+      <c r="BG3" s="40"/>
+      <c r="BH3" s="40"/>
+      <c r="BI3" s="40"/>
+      <c r="BJ3" s="40"/>
+      <c r="BK3" s="40"/>
+      <c r="BL3" s="40"/>
+      <c r="BM3" s="40"/>
+      <c r="BN3" s="40"/>
+    </row>
+    <row r="4" spans="1:66" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -1476,7 +1521,7 @@
       </c>
       <c r="G4" s="30"/>
     </row>
-    <row r="5" spans="1:66" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:66" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
@@ -1496,15 +1541,15 @@
         <v>1</v>
       </c>
       <c r="H5" s="30"/>
-      <c r="AC5" s="43"/>
-      <c r="AD5" s="43"/>
-      <c r="AE5" s="43"/>
-      <c r="AF5" s="43"/>
-      <c r="AG5" s="43"/>
-      <c r="AH5" s="43"/>
-      <c r="AI5" s="43"/>
-    </row>
-    <row r="6" spans="1:66" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AC5" s="36"/>
+      <c r="AD5" s="36"/>
+      <c r="AE5" s="36"/>
+      <c r="AF5" s="36"/>
+      <c r="AG5" s="36"/>
+      <c r="AH5" s="36"/>
+      <c r="AI5" s="36"/>
+    </row>
+    <row r="6" spans="1:66" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
@@ -1525,35 +1570,35 @@
       </c>
       <c r="H6" s="30"/>
       <c r="I6" s="31"/>
-      <c r="AC6" s="44"/>
-      <c r="AD6" s="45" t="s">
+      <c r="AC6" s="37"/>
+      <c r="AD6" s="48" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE6" s="50"/>
+      <c r="AF6" s="49"/>
+      <c r="AG6" s="48" t="s">
         <v>65</v>
       </c>
-      <c r="AE6" s="45"/>
-      <c r="AF6" s="45"/>
-      <c r="AG6" s="45" t="s">
-        <v>68</v>
-      </c>
-      <c r="AH6" s="45"/>
-      <c r="AI6" s="45"/>
-    </row>
-    <row r="7" spans="1:66" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AH6" s="50"/>
+      <c r="AI6" s="49"/>
+    </row>
+    <row r="7" spans="1:66" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="AC7" s="46"/>
-      <c r="AD7" s="45" t="s">
-        <v>64</v>
-      </c>
-      <c r="AE7" s="45"/>
-      <c r="AF7" s="45"/>
-      <c r="AG7" s="45" t="s">
-        <v>69</v>
-      </c>
-      <c r="AH7" s="45"/>
-      <c r="AI7" s="45"/>
-    </row>
-    <row r="8" spans="1:66" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+      <c r="AC7" s="38"/>
+      <c r="AD7" s="48" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE7" s="50"/>
+      <c r="AF7" s="49"/>
+      <c r="AG7" s="48" t="s">
+        <v>66</v>
+      </c>
+      <c r="AH7" s="50"/>
+      <c r="AI7" s="49"/>
+    </row>
+    <row r="8" spans="1:66" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>9</v>
       </c>
@@ -1575,19 +1620,19 @@
       <c r="H8" s="31"/>
       <c r="I8" s="29"/>
       <c r="J8" s="29"/>
-      <c r="AC8" s="47"/>
-      <c r="AD8" s="45" t="s">
-        <v>66</v>
-      </c>
-      <c r="AE8" s="45"/>
-      <c r="AF8" s="45"/>
-      <c r="AG8" s="45" t="s">
-        <v>70</v>
-      </c>
-      <c r="AH8" s="45"/>
-      <c r="AI8" s="45"/>
-    </row>
-    <row r="9" spans="1:66" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AC8" s="39"/>
+      <c r="AD8" s="48" t="s">
+        <v>63</v>
+      </c>
+      <c r="AE8" s="50"/>
+      <c r="AF8" s="49"/>
+      <c r="AG8" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="AH8" s="50"/>
+      <c r="AI8" s="49"/>
+    </row>
+    <row r="9" spans="1:66" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>10</v>
       </c>
@@ -1608,19 +1653,19 @@
       </c>
       <c r="J9" s="29"/>
       <c r="K9" s="31"/>
-      <c r="AC9" s="46"/>
-      <c r="AD9" s="44"/>
-      <c r="AE9" s="45" t="s">
-        <v>67</v>
-      </c>
-      <c r="AF9" s="45"/>
-      <c r="AG9" s="45" t="s">
-        <v>71</v>
-      </c>
-      <c r="AH9" s="45"/>
-      <c r="AI9" s="45"/>
-    </row>
-    <row r="10" spans="1:66" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AC9" s="38"/>
+      <c r="AD9" s="37"/>
+      <c r="AE9" s="48" t="s">
+        <v>64</v>
+      </c>
+      <c r="AF9" s="49"/>
+      <c r="AG9" s="48" t="s">
+        <v>68</v>
+      </c>
+      <c r="AH9" s="50"/>
+      <c r="AI9" s="49"/>
+    </row>
+    <row r="10" spans="1:66" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
         <v>11</v>
       </c>
@@ -1648,7 +1693,7 @@
       <c r="AH10" s="19"/>
       <c r="AI10" s="19"/>
     </row>
-    <row r="11" spans="1:66" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:66" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>12</v>
       </c>
@@ -1670,12 +1715,12 @@
       <c r="L11" s="29"/>
       <c r="M11" s="29"/>
     </row>
-    <row r="12" spans="1:66" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:66" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="12" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="13" spans="1:66" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:66" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
         <v>13</v>
       </c>
@@ -1694,10 +1739,10 @@
       <c r="F13" s="24">
         <v>1</v>
       </c>
-      <c r="K13" s="39"/>
+      <c r="K13" s="32"/>
       <c r="L13" s="31"/>
     </row>
-    <row r="14" spans="1:66" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:66" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
         <v>14</v>
       </c>
@@ -1714,13 +1759,13 @@
         <v>3</v>
       </c>
       <c r="F14" t="s">
-        <v>61</v>
-      </c>
-      <c r="L14" s="39"/>
-      <c r="M14" s="39"/>
+        <v>58</v>
+      </c>
+      <c r="L14" s="32"/>
+      <c r="M14" s="32"/>
       <c r="N14" s="31"/>
     </row>
-    <row r="15" spans="1:66" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:66" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
         <v>15</v>
       </c>
@@ -1737,12 +1782,12 @@
         <v>2</v>
       </c>
       <c r="F15" t="s">
-        <v>61</v>
-      </c>
-      <c r="M15" s="39"/>
+        <v>58</v>
+      </c>
+      <c r="M15" s="32"/>
       <c r="N15" s="31"/>
     </row>
-    <row r="16" spans="1:66" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:66" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
         <v>16</v>
       </c>
@@ -1759,18 +1804,18 @@
         <v>3</v>
       </c>
       <c r="F16" t="s">
-        <v>61</v>
-      </c>
-      <c r="M16" s="39"/>
-      <c r="N16" s="39"/>
+        <v>58</v>
+      </c>
+      <c r="M16" s="32"/>
+      <c r="N16" s="32"/>
       <c r="O16" s="31"/>
     </row>
-    <row r="17" spans="1:20" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:20" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="13" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="18" spans="1:20" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
         <v>17</v>
       </c>
@@ -1789,10 +1834,10 @@
       <c r="F18" s="24">
         <v>1</v>
       </c>
-      <c r="L18" s="40"/>
+      <c r="L18" s="33"/>
       <c r="M18" s="31"/>
     </row>
-    <row r="19" spans="1:20" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:20" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
         <v>18</v>
       </c>
@@ -1811,9 +1856,9 @@
       <c r="F19" s="24">
         <v>1</v>
       </c>
-      <c r="M19" s="40"/>
-    </row>
-    <row r="20" spans="1:20" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M19" s="33"/>
+    </row>
+    <row r="20" spans="1:20" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
         <v>19</v>
       </c>
@@ -1832,9 +1877,9 @@
       <c r="F20" s="24">
         <v>1</v>
       </c>
-      <c r="M20" s="40"/>
-    </row>
-    <row r="21" spans="1:20" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M20" s="33"/>
+    </row>
+    <row r="21" spans="1:20" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
         <v>20</v>
       </c>
@@ -1853,11 +1898,11 @@
       <c r="F21" s="24">
         <v>1</v>
       </c>
-      <c r="M21" s="40"/>
-      <c r="N21" s="40"/>
+      <c r="M21" s="33"/>
+      <c r="N21" s="33"/>
       <c r="O21" s="31"/>
     </row>
-    <row r="22" spans="1:20" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:20" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="s">
         <v>21</v>
       </c>
@@ -1876,17 +1921,17 @@
       <c r="F22" s="24">
         <v>1</v>
       </c>
-      <c r="N22" s="40"/>
-      <c r="O22" s="40"/>
-      <c r="P22" s="40"/>
+      <c r="N22" s="33"/>
+      <c r="O22" s="33"/>
+      <c r="P22" s="33"/>
       <c r="Q22" s="31"/>
     </row>
-    <row r="23" spans="1:20" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:20" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="13" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="24" spans="1:20" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="s">
         <v>22</v>
       </c>
@@ -1905,12 +1950,12 @@
       <c r="F24" s="24">
         <v>1</v>
       </c>
-      <c r="P24" s="41"/>
-      <c r="Q24" s="41"/>
+      <c r="P24" s="34"/>
+      <c r="Q24" s="34"/>
       <c r="R24" s="31"/>
       <c r="S24" s="31"/>
     </row>
-    <row r="25" spans="1:20" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:20" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="4" t="s">
         <v>23</v>
       </c>
@@ -1933,17 +1978,17 @@
       <c r="S25" s="31"/>
       <c r="T25" s="31"/>
     </row>
-    <row r="26" spans="1:20" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:20" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="13" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="27" spans="1:20" ht="17.25" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A27" s="25" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:20" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
         <v>25</v>
       </c>
@@ -1958,9 +2003,9 @@
       </c>
       <c r="N28" s="16"/>
     </row>
-    <row r="29" spans="1:20" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:20" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
-        <v>26</v>
+        <v>69</v>
       </c>
       <c r="B29">
         <v>9</v>
@@ -1974,9 +2019,9 @@
       <c r="O29" s="16"/>
       <c r="P29" s="16"/>
     </row>
-    <row r="30" spans="1:20" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:20" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B30">
         <v>10</v>
@@ -1991,9 +2036,9 @@
       <c r="Q30" s="16"/>
       <c r="R30" s="16"/>
     </row>
-    <row r="31" spans="1:20" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:20" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
-        <v>28</v>
+        <v>70</v>
       </c>
       <c r="B31">
         <v>11</v>
@@ -2009,9 +2054,9 @@
       <c r="S31" s="16"/>
       <c r="T31" s="16"/>
     </row>
-    <row r="32" spans="1:20" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:20" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
-        <v>29</v>
+        <v>71</v>
       </c>
       <c r="B32">
         <v>13</v>
@@ -2025,243 +2070,232 @@
       <c r="S32" s="16"/>
       <c r="T32" s="16"/>
     </row>
-    <row r="33" spans="1:29" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A33" s="26" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="34" spans="1:29" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B34">
+    <row r="33" spans="1:28" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A33" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B33">
+        <v>15</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+      <c r="F33" s="24">
+        <v>0</v>
+      </c>
+      <c r="S33" s="19"/>
+      <c r="T33" s="19"/>
+      <c r="U33" s="16"/>
+    </row>
+    <row r="34" spans="1:28" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A34" s="26" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="35" spans="1:28" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A35" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B35">
         <v>9</v>
       </c>
-      <c r="C34">
-        <v>1</v>
-      </c>
-      <c r="F34" s="24">
-        <v>0</v>
-      </c>
-      <c r="O34" s="16"/>
-    </row>
-    <row r="35" spans="1:29" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B35">
-        <v>10</v>
-      </c>
       <c r="C35">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F35" s="24">
         <v>0</v>
       </c>
-      <c r="P35" s="16"/>
-      <c r="Q35" s="16"/>
-    </row>
-    <row r="36" spans="1:29" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="O35" s="16"/>
+    </row>
+    <row r="36" spans="1:28" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B36">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C36">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F36" s="24">
         <v>0</v>
       </c>
+      <c r="P36" s="16"/>
       <c r="Q36" s="16"/>
-      <c r="R36" s="16"/>
-      <c r="S36" s="16"/>
-    </row>
-    <row r="37" spans="1:29" ht="17.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:28" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B37">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C37">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F37" s="24">
         <v>0</v>
       </c>
+      <c r="Q37" s="16"/>
+      <c r="R37" s="16"/>
       <c r="S37" s="16"/>
-      <c r="T37" s="16"/>
-    </row>
-    <row r="38" spans="1:29" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="38" spans="1:28" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B38">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C38">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F38" s="24">
         <v>0</v>
       </c>
-      <c r="R38" s="16"/>
       <c r="S38" s="16"/>
       <c r="T38" s="16"/>
-      <c r="U38" s="16"/>
-    </row>
-    <row r="39" spans="1:29" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="13" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="40" spans="1:29" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B40">
+    </row>
+    <row r="39" spans="1:28" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B39">
+        <v>12</v>
+      </c>
+      <c r="C39">
+        <v>4</v>
+      </c>
+      <c r="F39" s="24">
+        <v>0</v>
+      </c>
+      <c r="R39" s="16"/>
+      <c r="S39" s="16"/>
+      <c r="T39" s="16"/>
+      <c r="U39" s="16"/>
+    </row>
+    <row r="40" spans="1:28" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="41" spans="1:28" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A41" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B41">
         <v>14</v>
       </c>
-      <c r="C40">
+      <c r="C41">
         <v>3</v>
-      </c>
-      <c r="F40" s="24">
-        <v>0</v>
-      </c>
-      <c r="T40" s="17"/>
-      <c r="U40" s="17"/>
-      <c r="V40" s="17"/>
-    </row>
-    <row r="41" spans="1:29" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A41" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B41">
-        <v>16</v>
-      </c>
-      <c r="C41">
-        <v>1</v>
       </c>
       <c r="F41" s="24">
         <v>0</v>
       </c>
+      <c r="T41" s="17"/>
+      <c r="U41" s="17"/>
       <c r="V41" s="17"/>
     </row>
-    <row r="42" spans="1:29" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:28" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B42">
         <v>16</v>
       </c>
       <c r="C42">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F42" s="24">
         <v>0</v>
       </c>
       <c r="V42" s="17"/>
-      <c r="W42" s="17"/>
-    </row>
-    <row r="43" spans="1:29" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="43" spans="1:28" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B43">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C43">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F43" s="24">
         <v>0</v>
       </c>
-      <c r="X43" s="17"/>
-    </row>
-    <row r="44" spans="1:29" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="N44" s="19"/>
-      <c r="O44" s="19"/>
-      <c r="P44" s="19"/>
-      <c r="Q44" s="19"/>
-      <c r="R44" s="19"/>
-      <c r="S44" s="19"/>
-      <c r="T44" s="19"/>
-      <c r="U44" s="19"/>
-      <c r="V44" s="19"/>
-      <c r="W44" s="19"/>
-      <c r="X44" s="19"/>
-      <c r="Y44" s="19"/>
-      <c r="Z44" s="19"/>
-    </row>
-    <row r="45" spans="1:29" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A45" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B45">
-        <v>13</v>
-      </c>
-      <c r="C45">
-        <v>7</v>
-      </c>
-      <c r="F45" s="24">
+      <c r="V43" s="17"/>
+      <c r="W43" s="17"/>
+    </row>
+    <row r="44" spans="1:28" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B44">
+        <v>18</v>
+      </c>
+      <c r="C44">
+        <v>1</v>
+      </c>
+      <c r="F44" s="24">
         <v>0</v>
+      </c>
+      <c r="X44" s="17"/>
+    </row>
+    <row r="45" spans="1:28" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="13" t="s">
+        <v>56</v>
       </c>
       <c r="N45" s="19"/>
       <c r="O45" s="19"/>
-      <c r="P45" s="20"/>
-      <c r="Q45" s="20"/>
-      <c r="R45" s="20"/>
-      <c r="S45" s="21"/>
-      <c r="T45" s="21"/>
-      <c r="U45" s="21"/>
-      <c r="V45" s="21"/>
-      <c r="W45" s="21"/>
-      <c r="X45" s="21"/>
-      <c r="Y45" s="21"/>
+      <c r="P45" s="19"/>
+      <c r="Q45" s="19"/>
+      <c r="R45" s="19"/>
+      <c r="S45" s="19"/>
+      <c r="T45" s="19"/>
+      <c r="U45" s="19"/>
+      <c r="V45" s="19"/>
+      <c r="W45" s="19"/>
+      <c r="X45" s="19"/>
+      <c r="Y45" s="19"/>
       <c r="Z45" s="19"/>
     </row>
-    <row r="46" spans="1:29" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A46" s="6" t="s">
-        <v>41</v>
+    <row r="46" spans="1:28" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A46" s="5" t="s">
+        <v>37</v>
       </c>
       <c r="B46">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C46">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F46" s="24">
         <v>0</v>
       </c>
       <c r="N46" s="19"/>
       <c r="O46" s="19"/>
-      <c r="P46" s="19"/>
-      <c r="Q46" s="19"/>
-      <c r="R46" s="19"/>
-      <c r="S46" s="19"/>
-      <c r="T46" s="19"/>
-      <c r="U46" s="19"/>
-      <c r="V46" s="19"/>
-      <c r="W46" s="18"/>
-      <c r="X46" s="18"/>
-      <c r="Y46" s="18"/>
-      <c r="Z46" s="18"/>
-      <c r="AA46" s="18"/>
-    </row>
-    <row r="47" spans="1:29" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A47" s="5" t="s">
-        <v>42</v>
+      <c r="P46" s="20"/>
+      <c r="Q46" s="20"/>
+      <c r="R46" s="20"/>
+      <c r="S46" s="21"/>
+      <c r="T46" s="21"/>
+      <c r="U46" s="21"/>
+      <c r="V46" s="21"/>
+      <c r="W46" s="21"/>
+      <c r="X46" s="21"/>
+      <c r="Y46" s="21"/>
+      <c r="Z46" s="19"/>
+    </row>
+    <row r="47" spans="1:28" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A47" s="6" t="s">
+        <v>38</v>
       </c>
       <c r="B47">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C47">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F47" s="24">
         <v>0</v>
@@ -2275,195 +2309,192 @@
       <c r="T47" s="19"/>
       <c r="U47" s="19"/>
       <c r="V47" s="19"/>
-      <c r="W47" s="19"/>
-      <c r="X47" s="19"/>
-      <c r="Y47" s="19"/>
+      <c r="W47" s="18"/>
+      <c r="X47" s="18"/>
+      <c r="Y47" s="18"/>
       <c r="Z47" s="18"/>
       <c r="AA47" s="18"/>
-      <c r="AB47" s="18"/>
-    </row>
-    <row r="48" spans="1:29" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="48" spans="1:28" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B48">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C48">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F48" s="24">
         <v>0</v>
       </c>
-      <c r="AC48" s="18"/>
-    </row>
-    <row r="49" spans="1:35" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="13" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="50" spans="1:35" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="B50">
+      <c r="N48" s="19"/>
+      <c r="O48" s="19"/>
+      <c r="P48" s="19"/>
+      <c r="Q48" s="19"/>
+      <c r="R48" s="19"/>
+      <c r="S48" s="19"/>
+      <c r="T48" s="19"/>
+      <c r="U48" s="19"/>
+      <c r="V48" s="19"/>
+      <c r="W48" s="19"/>
+      <c r="X48" s="19"/>
+      <c r="Y48" s="19"/>
+      <c r="Z48" s="18"/>
+      <c r="AA48" s="18"/>
+      <c r="AB48" s="18"/>
+    </row>
+    <row r="49" spans="1:35" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B49">
+        <v>23</v>
+      </c>
+      <c r="C49">
+        <v>1</v>
+      </c>
+      <c r="F49" s="24">
+        <v>0</v>
+      </c>
+      <c r="AC49" s="18"/>
+    </row>
+    <row r="50" spans="1:35" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="51" spans="1:35" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B51">
         <v>9</v>
       </c>
-      <c r="C50">
+      <c r="C51">
         <v>7</v>
       </c>
-      <c r="D50">
+      <c r="D51">
         <v>9</v>
       </c>
-      <c r="E50">
+      <c r="E51">
         <v>7</v>
       </c>
-      <c r="F50" t="s">
-        <v>61</v>
-      </c>
-      <c r="O50" s="42"/>
-      <c r="P50" s="42"/>
-      <c r="Q50" s="42"/>
-      <c r="R50" s="42"/>
-      <c r="S50" s="42"/>
-      <c r="T50" s="42"/>
-      <c r="U50" s="42"/>
-      <c r="V50" s="19"/>
-      <c r="W50" s="19"/>
-      <c r="X50" s="19"/>
-      <c r="Y50" s="19"/>
-      <c r="Z50" s="19"/>
-      <c r="AA50" s="28"/>
-      <c r="AB50" s="28"/>
-      <c r="AC50" s="28"/>
-      <c r="AD50" s="22"/>
-      <c r="AE50" s="22"/>
-    </row>
-    <row r="51" spans="1:35" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="B51">
+      <c r="F51" t="s">
+        <v>58</v>
+      </c>
+      <c r="O51" s="35"/>
+      <c r="P51" s="35"/>
+      <c r="Q51" s="35"/>
+      <c r="R51" s="35"/>
+      <c r="S51" s="35"/>
+      <c r="T51" s="35"/>
+      <c r="U51" s="35"/>
+      <c r="V51" s="19"/>
+      <c r="W51" s="19"/>
+      <c r="X51" s="19"/>
+      <c r="Y51" s="19"/>
+      <c r="Z51" s="19"/>
+      <c r="AA51" s="28"/>
+      <c r="AB51" s="28"/>
+      <c r="AC51" s="28"/>
+      <c r="AD51" s="22"/>
+      <c r="AE51" s="22"/>
+    </row>
+    <row r="52" spans="1:35" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B52">
         <v>13</v>
       </c>
-      <c r="C51">
+      <c r="C52">
         <v>3</v>
       </c>
-      <c r="D51">
+      <c r="D52">
         <v>13</v>
       </c>
-      <c r="E51">
+      <c r="E52">
         <v>3</v>
       </c>
-      <c r="F51" t="s">
-        <v>61</v>
-      </c>
-      <c r="S51" s="42"/>
-      <c r="T51" s="42"/>
-      <c r="U51" s="42"/>
-      <c r="AA51" s="19"/>
-      <c r="AB51" s="19"/>
-      <c r="AC51" s="19"/>
-      <c r="AD51" s="28"/>
-      <c r="AE51" s="22"/>
-      <c r="AF51" s="22"/>
-    </row>
-    <row r="52" spans="1:35" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="B52">
-        <v>15</v>
-      </c>
-      <c r="C52">
-        <v>1</v>
-      </c>
-      <c r="D52">
-        <v>15</v>
-      </c>
-      <c r="E52">
-        <v>1</v>
-      </c>
       <c r="F52" t="s">
-        <v>61</v>
-      </c>
-      <c r="U52" s="42"/>
-      <c r="AD52" s="19"/>
+        <v>58</v>
+      </c>
+      <c r="S52" s="35"/>
+      <c r="T52" s="35"/>
+      <c r="U52" s="35"/>
+      <c r="AA52" s="19"/>
+      <c r="AB52" s="19"/>
+      <c r="AC52" s="19"/>
+      <c r="AD52" s="28"/>
       <c r="AE52" s="22"/>
       <c r="AF52" s="22"/>
     </row>
-    <row r="53" spans="1:35" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:35" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A53" s="5" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B53">
+        <v>15</v>
+      </c>
+      <c r="C53">
+        <v>1</v>
+      </c>
+      <c r="D53">
+        <v>15</v>
+      </c>
+      <c r="E53">
+        <v>1</v>
+      </c>
+      <c r="F53" t="s">
+        <v>58</v>
+      </c>
+      <c r="U53" s="35"/>
+      <c r="AD53" s="19"/>
+      <c r="AE53" s="22"/>
+      <c r="AF53" s="22"/>
+    </row>
+    <row r="54" spans="1:35" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A54" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B54">
         <v>10</v>
       </c>
-      <c r="C53">
+      <c r="C54">
         <v>6</v>
       </c>
-      <c r="D53">
+      <c r="D54">
         <v>10</v>
       </c>
-      <c r="E53">
+      <c r="E54">
         <v>6</v>
       </c>
-      <c r="F53" t="s">
-        <v>61</v>
-      </c>
-      <c r="P53" s="42"/>
-      <c r="Q53" s="42"/>
-      <c r="R53" s="42"/>
-      <c r="S53" s="42"/>
-      <c r="T53" s="42"/>
-      <c r="U53" s="42"/>
-      <c r="V53" s="19"/>
-      <c r="W53" s="19"/>
-      <c r="X53" s="19"/>
-      <c r="Y53" s="19"/>
-      <c r="Z53" s="19"/>
-      <c r="AA53" s="28"/>
-      <c r="AB53" s="28"/>
-      <c r="AC53" s="28"/>
-      <c r="AD53" s="28"/>
-      <c r="AE53" s="28"/>
-      <c r="AF53" s="28"/>
-      <c r="AG53" s="28"/>
-    </row>
-    <row r="54" spans="1:35" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B54">
-        <v>15</v>
-      </c>
-      <c r="C54">
-        <v>1</v>
-      </c>
-      <c r="D54">
-        <v>15</v>
-      </c>
-      <c r="E54">
-        <v>1</v>
-      </c>
       <c r="F54" t="s">
-        <v>61</v>
-      </c>
-      <c r="U54" s="42"/>
+        <v>58</v>
+      </c>
+      <c r="P54" s="35"/>
+      <c r="Q54" s="35"/>
+      <c r="R54" s="35"/>
+      <c r="S54" s="35"/>
+      <c r="T54" s="35"/>
+      <c r="U54" s="35"/>
+      <c r="V54" s="19"/>
+      <c r="W54" s="19"/>
       <c r="X54" s="19"/>
       <c r="Y54" s="19"/>
       <c r="Z54" s="19"/>
-      <c r="AA54" s="19"/>
-      <c r="AB54" s="19"/>
-      <c r="AC54" s="19"/>
-      <c r="AD54" s="19"/>
+      <c r="AA54" s="28"/>
+      <c r="AB54" s="28"/>
+      <c r="AC54" s="28"/>
+      <c r="AD54" s="28"/>
       <c r="AE54" s="28"/>
       <c r="AF54" s="28"/>
-      <c r="AG54" s="22"/>
-    </row>
-    <row r="55" spans="1:35" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AG54" s="28"/>
+    </row>
+    <row r="55" spans="1:35" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A55" s="5" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B55">
         <v>15</v>
@@ -2475,60 +2506,67 @@
         <v>15</v>
       </c>
       <c r="E55">
+        <v>1</v>
+      </c>
+      <c r="F55" t="s">
+        <v>58</v>
+      </c>
+      <c r="U55" s="35"/>
+      <c r="X55" s="19"/>
+      <c r="Y55" s="19"/>
+      <c r="Z55" s="19"/>
+      <c r="AA55" s="19"/>
+      <c r="AB55" s="19"/>
+      <c r="AC55" s="19"/>
+      <c r="AD55" s="19"/>
+      <c r="AE55" s="28"/>
+      <c r="AF55" s="28"/>
+      <c r="AG55" s="22"/>
+    </row>
+    <row r="56" spans="1:35" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A56" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B56">
+        <v>15</v>
+      </c>
+      <c r="C56">
+        <v>1</v>
+      </c>
+      <c r="D56">
+        <v>15</v>
+      </c>
+      <c r="E56">
         <v>2</v>
       </c>
-      <c r="F55" t="s">
-        <v>61</v>
-      </c>
-      <c r="U55" s="42"/>
-      <c r="V55" s="31"/>
-      <c r="AD55" s="19"/>
-      <c r="AE55" s="19"/>
-      <c r="AF55" s="19"/>
-      <c r="AG55" s="22"/>
-      <c r="AH55" s="22"/>
-    </row>
-    <row r="56" spans="1:35" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="13" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="57" spans="1:35" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B57">
+      <c r="F56" t="s">
+        <v>58</v>
+      </c>
+      <c r="U56" s="35"/>
+      <c r="V56" s="31"/>
+      <c r="AD56" s="19"/>
+      <c r="AE56" s="19"/>
+      <c r="AF56" s="19"/>
+      <c r="AG56" s="22"/>
+      <c r="AH56" s="22"/>
+    </row>
+    <row r="57" spans="1:35" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A57" s="13" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="58" spans="1:35" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A58" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B58">
         <v>15</v>
       </c>
-      <c r="C57">
+      <c r="C58">
         <v>2</v>
       </c>
-      <c r="D57">
+      <c r="D58">
         <v>16</v>
-      </c>
-      <c r="E57">
-        <v>1</v>
-      </c>
-      <c r="F57" s="24">
-        <v>0.5</v>
-      </c>
-      <c r="U57" s="14"/>
-      <c r="V57" s="31"/>
-      <c r="AH57" s="23"/>
-      <c r="AI57" s="23"/>
-    </row>
-    <row r="58" spans="1:35" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="B58">
-        <v>16</v>
-      </c>
-      <c r="C58">
-        <v>1</v>
-      </c>
-      <c r="D58">
-        <v>17</v>
       </c>
       <c r="E58">
         <v>1</v>
@@ -2536,13 +2574,45 @@
       <c r="F58" s="24">
         <v>0.5</v>
       </c>
-      <c r="V58" s="14"/>
-      <c r="W58" s="31"/>
+      <c r="U58" s="14"/>
+      <c r="V58" s="31"/>
+      <c r="AH58" s="23"/>
       <c r="AI58" s="23"/>
     </row>
-    <row r="59" spans="1:35" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="59" spans="1:35" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A59" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B59">
+        <v>16</v>
+      </c>
+      <c r="C59">
+        <v>1</v>
+      </c>
+      <c r="D59">
+        <v>17</v>
+      </c>
+      <c r="E59">
+        <v>1</v>
+      </c>
+      <c r="F59" s="24">
+        <v>0.5</v>
+      </c>
+      <c r="V59" s="14"/>
+      <c r="W59" s="31"/>
+      <c r="AI59" s="23"/>
+    </row>
+    <row r="60" spans="1:35" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="G1:AI1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
     <mergeCell ref="AG6:AI6"/>
     <mergeCell ref="AG7:AI7"/>
     <mergeCell ref="AG8:AI8"/>
@@ -2551,14 +2621,6 @@
     <mergeCell ref="AD8:AF8"/>
     <mergeCell ref="AD7:AF7"/>
     <mergeCell ref="AE9:AF9"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="G1:AI1"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
   </mergeCells>
   <conditionalFormatting sqref="G2:BN3">
     <cfRule type="expression" dxfId="0" priority="1">

</xml_diff>

<commit_message>
1st Update to Gantt Chart
</commit_message>
<xml_diff>
--- a/Gantt chart.xlsx
+++ b/Gantt chart.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26731"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pranj\software-tech-ass\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avaiv\software-tech-ass\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C900504-1309-4D1F-9259-A166D908B309}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BCF5635-4AC9-40DE-8CF0-68C7FB3D383B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-1635" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="79">
   <si>
     <t>ACTIVITY</t>
   </si>
@@ -263,6 +263,24 @@
   </si>
   <si>
     <t>Data visualization</t>
+  </si>
+  <si>
+    <t>Test Data Visualization features</t>
+  </si>
+  <si>
+    <t>Prepare a User Manual</t>
+  </si>
+  <si>
+    <t>Data Analysis and Reporting</t>
+  </si>
+  <si>
+    <t>Perform Data Analysis over a 12 month period</t>
+  </si>
+  <si>
+    <t>Create an Executive Summary</t>
+  </si>
+  <si>
+    <t>12 Months</t>
   </si>
 </sst>
 </file>
@@ -763,7 +781,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -911,11 +929,14 @@
     <xf numFmtId="0" fontId="15" fillId="26" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="26" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="26" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="26" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -1203,10 +1224,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BN60"/>
+  <dimension ref="A1:BN64"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="30" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AJ59" sqref="A1:AJ59"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P71" sqref="P71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1574,13 +1595,13 @@
       <c r="AD6" s="48" t="s">
         <v>62</v>
       </c>
-      <c r="AE6" s="50"/>
-      <c r="AF6" s="49"/>
+      <c r="AE6" s="49"/>
+      <c r="AF6" s="50"/>
       <c r="AG6" s="48" t="s">
         <v>65</v>
       </c>
-      <c r="AH6" s="50"/>
-      <c r="AI6" s="49"/>
+      <c r="AH6" s="49"/>
+      <c r="AI6" s="50"/>
     </row>
     <row r="7" spans="1:66" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="11" t="s">
@@ -1590,13 +1611,13 @@
       <c r="AD7" s="48" t="s">
         <v>61</v>
       </c>
-      <c r="AE7" s="50"/>
-      <c r="AF7" s="49"/>
+      <c r="AE7" s="49"/>
+      <c r="AF7" s="50"/>
       <c r="AG7" s="48" t="s">
         <v>66</v>
       </c>
-      <c r="AH7" s="50"/>
-      <c r="AI7" s="49"/>
+      <c r="AH7" s="49"/>
+      <c r="AI7" s="50"/>
     </row>
     <row r="8" spans="1:66" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
@@ -1624,13 +1645,13 @@
       <c r="AD8" s="48" t="s">
         <v>63</v>
       </c>
-      <c r="AE8" s="50"/>
-      <c r="AF8" s="49"/>
+      <c r="AE8" s="49"/>
+      <c r="AF8" s="50"/>
       <c r="AG8" s="48" t="s">
         <v>67</v>
       </c>
-      <c r="AH8" s="50"/>
-      <c r="AI8" s="49"/>
+      <c r="AH8" s="49"/>
+      <c r="AI8" s="50"/>
     </row>
     <row r="9" spans="1:66" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
@@ -1658,12 +1679,12 @@
       <c r="AE9" s="48" t="s">
         <v>64</v>
       </c>
-      <c r="AF9" s="49"/>
+      <c r="AF9" s="50"/>
       <c r="AG9" s="48" t="s">
         <v>68</v>
       </c>
-      <c r="AH9" s="50"/>
-      <c r="AI9" s="49"/>
+      <c r="AH9" s="49"/>
+      <c r="AI9" s="50"/>
     </row>
     <row r="10" spans="1:66" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
@@ -2070,7 +2091,7 @@
       <c r="S32" s="16"/>
       <c r="T32" s="16"/>
     </row>
-    <row r="33" spans="1:28" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
         <v>72</v>
       </c>
@@ -2087,12 +2108,12 @@
       <c r="T33" s="19"/>
       <c r="U33" s="16"/>
     </row>
-    <row r="34" spans="1:28" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A34" s="26" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="35" spans="1:28" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
         <v>28</v>
       </c>
@@ -2107,7 +2128,7 @@
       </c>
       <c r="O35" s="16"/>
     </row>
-    <row r="36" spans="1:28" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
         <v>29</v>
       </c>
@@ -2123,182 +2144,150 @@
       <c r="P36" s="16"/>
       <c r="Q36" s="16"/>
     </row>
-    <row r="37" spans="1:28" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
-        <v>30</v>
+        <v>73</v>
       </c>
       <c r="B37">
         <v>11</v>
       </c>
       <c r="C37">
-        <v>3</v>
-      </c>
-      <c r="F37" s="24">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q37" s="16"/>
       <c r="R37" s="16"/>
-      <c r="S37" s="16"/>
-    </row>
-    <row r="38" spans="1:28" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    </row>
+    <row r="38" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B38">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C38">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F38" s="24">
         <v>0</v>
       </c>
+      <c r="Q38" s="16"/>
+      <c r="R38" s="16"/>
       <c r="S38" s="16"/>
-      <c r="T38" s="16"/>
-    </row>
-    <row r="39" spans="1:28" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="39" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B39">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C39">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F39" s="24">
         <v>0</v>
       </c>
-      <c r="R39" s="16"/>
       <c r="S39" s="16"/>
       <c r="T39" s="16"/>
-      <c r="U39" s="16"/>
-    </row>
-    <row r="40" spans="1:28" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="13" t="s">
+    </row>
+    <row r="40" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B40">
+        <v>12</v>
+      </c>
+      <c r="C40">
+        <v>4</v>
+      </c>
+      <c r="F40" s="24">
+        <v>0</v>
+      </c>
+      <c r="R40" s="16"/>
+      <c r="S40" s="16"/>
+      <c r="T40" s="16"/>
+      <c r="U40" s="16"/>
+    </row>
+    <row r="41" spans="1:26" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="13" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="41" spans="1:28" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A41" s="3" t="s">
+    <row r="42" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A42" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B41">
+      <c r="B42">
         <v>14</v>
       </c>
-      <c r="C41">
+      <c r="C42">
         <v>3</v>
-      </c>
-      <c r="F41" s="24">
-        <v>0</v>
-      </c>
-      <c r="T41" s="17"/>
-      <c r="U41" s="17"/>
-      <c r="V41" s="17"/>
-    </row>
-    <row r="42" spans="1:28" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A42" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B42">
-        <v>16</v>
-      </c>
-      <c r="C42">
-        <v>1</v>
       </c>
       <c r="F42" s="24">
         <v>0</v>
       </c>
+      <c r="T42" s="17"/>
+      <c r="U42" s="17"/>
       <c r="V42" s="17"/>
     </row>
-    <row r="43" spans="1:28" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B43">
         <v>16</v>
       </c>
       <c r="C43">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F43" s="24">
         <v>0</v>
       </c>
       <c r="V43" s="17"/>
-      <c r="W43" s="17"/>
-    </row>
-    <row r="44" spans="1:28" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="44" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B44">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C44">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F44" s="24">
         <v>0</v>
       </c>
-      <c r="X44" s="17"/>
-    </row>
-    <row r="45" spans="1:28" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="13" t="s">
+      <c r="V44" s="17"/>
+      <c r="W44" s="17"/>
+    </row>
+    <row r="45" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A45" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B45">
+        <v>18</v>
+      </c>
+      <c r="C45">
+        <v>1</v>
+      </c>
+      <c r="F45" s="24">
+        <v>0</v>
+      </c>
+      <c r="X45" s="17"/>
+    </row>
+    <row r="46" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="51" t="s">
+        <v>74</v>
+      </c>
+      <c r="C46">
+        <v>2</v>
+      </c>
+      <c r="Y46" s="17"/>
+    </row>
+    <row r="47" spans="1:26" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="13" t="s">
         <v>56</v>
-      </c>
-      <c r="N45" s="19"/>
-      <c r="O45" s="19"/>
-      <c r="P45" s="19"/>
-      <c r="Q45" s="19"/>
-      <c r="R45" s="19"/>
-      <c r="S45" s="19"/>
-      <c r="T45" s="19"/>
-      <c r="U45" s="19"/>
-      <c r="V45" s="19"/>
-      <c r="W45" s="19"/>
-      <c r="X45" s="19"/>
-      <c r="Y45" s="19"/>
-      <c r="Z45" s="19"/>
-    </row>
-    <row r="46" spans="1:28" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A46" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B46">
-        <v>13</v>
-      </c>
-      <c r="C46">
-        <v>7</v>
-      </c>
-      <c r="F46" s="24">
-        <v>0</v>
-      </c>
-      <c r="N46" s="19"/>
-      <c r="O46" s="19"/>
-      <c r="P46" s="20"/>
-      <c r="Q46" s="20"/>
-      <c r="R46" s="20"/>
-      <c r="S46" s="21"/>
-      <c r="T46" s="21"/>
-      <c r="U46" s="21"/>
-      <c r="V46" s="21"/>
-      <c r="W46" s="21"/>
-      <c r="X46" s="21"/>
-      <c r="Y46" s="21"/>
-      <c r="Z46" s="19"/>
-    </row>
-    <row r="47" spans="1:28" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A47" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="B47">
-        <v>17</v>
-      </c>
-      <c r="C47">
-        <v>5</v>
-      </c>
-      <c r="F47" s="24">
-        <v>0</v>
       </c>
       <c r="N47" s="19"/>
       <c r="O47" s="19"/>
@@ -2309,192 +2298,184 @@
       <c r="T47" s="19"/>
       <c r="U47" s="19"/>
       <c r="V47" s="19"/>
-      <c r="W47" s="18"/>
-      <c r="X47" s="18"/>
-      <c r="Y47" s="18"/>
-      <c r="Z47" s="18"/>
-      <c r="AA47" s="18"/>
-    </row>
-    <row r="48" spans="1:28" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="W47" s="19"/>
+      <c r="X47" s="19"/>
+      <c r="Y47" s="19"/>
+      <c r="Z47" s="19"/>
+    </row>
+    <row r="48" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B48">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C48">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="F48" s="24">
         <v>0</v>
       </c>
       <c r="N48" s="19"/>
       <c r="O48" s="19"/>
-      <c r="P48" s="19"/>
-      <c r="Q48" s="19"/>
-      <c r="R48" s="19"/>
-      <c r="S48" s="19"/>
-      <c r="T48" s="19"/>
-      <c r="U48" s="19"/>
-      <c r="V48" s="19"/>
-      <c r="W48" s="19"/>
-      <c r="X48" s="19"/>
-      <c r="Y48" s="19"/>
-      <c r="Z48" s="18"/>
-      <c r="AA48" s="18"/>
-      <c r="AB48" s="18"/>
-    </row>
-    <row r="49" spans="1:35" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="5" t="s">
-        <v>40</v>
+      <c r="P48" s="20"/>
+      <c r="Q48" s="20"/>
+      <c r="R48" s="20"/>
+      <c r="S48" s="21"/>
+      <c r="T48" s="21"/>
+      <c r="U48" s="21"/>
+      <c r="V48" s="21"/>
+      <c r="W48" s="21"/>
+      <c r="X48" s="21"/>
+      <c r="Y48" s="21"/>
+      <c r="Z48" s="19"/>
+    </row>
+    <row r="49" spans="1:35" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A49" s="6" t="s">
+        <v>38</v>
       </c>
       <c r="B49">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C49">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F49" s="24">
         <v>0</v>
       </c>
-      <c r="AC49" s="18"/>
-    </row>
-    <row r="50" spans="1:35" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="13" t="s">
+      <c r="N49" s="19"/>
+      <c r="O49" s="19"/>
+      <c r="P49" s="19"/>
+      <c r="Q49" s="19"/>
+      <c r="R49" s="19"/>
+      <c r="S49" s="19"/>
+      <c r="T49" s="19"/>
+      <c r="U49" s="19"/>
+      <c r="V49" s="19"/>
+      <c r="W49" s="18"/>
+      <c r="X49" s="18"/>
+      <c r="Y49" s="18"/>
+      <c r="Z49" s="18"/>
+      <c r="AA49" s="18"/>
+    </row>
+    <row r="50" spans="1:35" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A50" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B50">
+        <v>20</v>
+      </c>
+      <c r="C50">
+        <v>3</v>
+      </c>
+      <c r="F50" s="24">
+        <v>0</v>
+      </c>
+      <c r="N50" s="19"/>
+      <c r="O50" s="19"/>
+      <c r="P50" s="19"/>
+      <c r="Q50" s="19"/>
+      <c r="R50" s="19"/>
+      <c r="S50" s="19"/>
+      <c r="T50" s="19"/>
+      <c r="U50" s="19"/>
+      <c r="V50" s="19"/>
+      <c r="W50" s="19"/>
+      <c r="X50" s="19"/>
+      <c r="Y50" s="19"/>
+      <c r="Z50" s="18"/>
+      <c r="AA50" s="18"/>
+      <c r="AB50" s="18"/>
+    </row>
+    <row r="51" spans="1:35" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B51">
+        <v>23</v>
+      </c>
+      <c r="C51">
+        <v>1</v>
+      </c>
+      <c r="F51" s="24">
+        <v>0</v>
+      </c>
+      <c r="AC51" s="18"/>
+    </row>
+    <row r="52" spans="1:35" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="13" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="51" spans="1:35" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="7" t="s">
+    <row r="53" spans="1:35" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="B51">
+      <c r="B53">
         <v>9</v>
       </c>
-      <c r="C51">
+      <c r="C53">
         <v>7</v>
       </c>
-      <c r="D51">
+      <c r="D53">
         <v>9</v>
       </c>
-      <c r="E51">
+      <c r="E53">
         <v>7</v>
-      </c>
-      <c r="F51" t="s">
-        <v>58</v>
-      </c>
-      <c r="O51" s="35"/>
-      <c r="P51" s="35"/>
-      <c r="Q51" s="35"/>
-      <c r="R51" s="35"/>
-      <c r="S51" s="35"/>
-      <c r="T51" s="35"/>
-      <c r="U51" s="35"/>
-      <c r="V51" s="19"/>
-      <c r="W51" s="19"/>
-      <c r="X51" s="19"/>
-      <c r="Y51" s="19"/>
-      <c r="Z51" s="19"/>
-      <c r="AA51" s="28"/>
-      <c r="AB51" s="28"/>
-      <c r="AC51" s="28"/>
-      <c r="AD51" s="22"/>
-      <c r="AE51" s="22"/>
-    </row>
-    <row r="52" spans="1:35" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="B52">
-        <v>13</v>
-      </c>
-      <c r="C52">
-        <v>3</v>
-      </c>
-      <c r="D52">
-        <v>13</v>
-      </c>
-      <c r="E52">
-        <v>3</v>
-      </c>
-      <c r="F52" t="s">
-        <v>58</v>
-      </c>
-      <c r="S52" s="35"/>
-      <c r="T52" s="35"/>
-      <c r="U52" s="35"/>
-      <c r="AA52" s="19"/>
-      <c r="AB52" s="19"/>
-      <c r="AC52" s="19"/>
-      <c r="AD52" s="28"/>
-      <c r="AE52" s="22"/>
-      <c r="AF52" s="22"/>
-    </row>
-    <row r="53" spans="1:35" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B53">
-        <v>15</v>
-      </c>
-      <c r="C53">
-        <v>1</v>
-      </c>
-      <c r="D53">
-        <v>15</v>
-      </c>
-      <c r="E53">
-        <v>1</v>
       </c>
       <c r="F53" t="s">
         <v>58</v>
       </c>
+      <c r="O53" s="35"/>
+      <c r="P53" s="35"/>
+      <c r="Q53" s="35"/>
+      <c r="R53" s="35"/>
+      <c r="S53" s="35"/>
+      <c r="T53" s="35"/>
       <c r="U53" s="35"/>
-      <c r="AD53" s="19"/>
+      <c r="V53" s="19"/>
+      <c r="W53" s="19"/>
+      <c r="X53" s="19"/>
+      <c r="Y53" s="19"/>
+      <c r="Z53" s="19"/>
+      <c r="AA53" s="28"/>
+      <c r="AB53" s="28"/>
+      <c r="AC53" s="28"/>
+      <c r="AD53" s="22"/>
       <c r="AE53" s="22"/>
-      <c r="AF53" s="22"/>
     </row>
     <row r="54" spans="1:35" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A54" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B54">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C54">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D54">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E54">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F54" t="s">
         <v>58</v>
       </c>
-      <c r="P54" s="35"/>
-      <c r="Q54" s="35"/>
-      <c r="R54" s="35"/>
       <c r="S54" s="35"/>
       <c r="T54" s="35"/>
       <c r="U54" s="35"/>
-      <c r="V54" s="19"/>
-      <c r="W54" s="19"/>
-      <c r="X54" s="19"/>
-      <c r="Y54" s="19"/>
-      <c r="Z54" s="19"/>
-      <c r="AA54" s="28"/>
-      <c r="AB54" s="28"/>
-      <c r="AC54" s="28"/>
+      <c r="AA54" s="19"/>
+      <c r="AB54" s="19"/>
+      <c r="AC54" s="19"/>
       <c r="AD54" s="28"/>
-      <c r="AE54" s="28"/>
-      <c r="AF54" s="28"/>
-      <c r="AG54" s="28"/>
+      <c r="AE54" s="22"/>
+      <c r="AF54" s="22"/>
     </row>
     <row r="55" spans="1:35" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A55" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B55">
         <v>15</v>
@@ -2512,99 +2493,191 @@
         <v>58</v>
       </c>
       <c r="U55" s="35"/>
-      <c r="X55" s="19"/>
-      <c r="Y55" s="19"/>
-      <c r="Z55" s="19"/>
-      <c r="AA55" s="19"/>
-      <c r="AB55" s="19"/>
-      <c r="AC55" s="19"/>
       <c r="AD55" s="19"/>
-      <c r="AE55" s="28"/>
-      <c r="AF55" s="28"/>
-      <c r="AG55" s="22"/>
+      <c r="AE55" s="22"/>
+      <c r="AF55" s="22"/>
     </row>
     <row r="56" spans="1:35" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A56" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B56">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C56">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D56">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E56">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F56" t="s">
         <v>58</v>
       </c>
+      <c r="P56" s="35"/>
+      <c r="Q56" s="35"/>
+      <c r="R56" s="35"/>
+      <c r="S56" s="35"/>
+      <c r="T56" s="35"/>
       <c r="U56" s="35"/>
-      <c r="V56" s="31"/>
-      <c r="AD56" s="19"/>
-      <c r="AE56" s="19"/>
-      <c r="AF56" s="19"/>
-      <c r="AG56" s="22"/>
-      <c r="AH56" s="22"/>
-    </row>
-    <row r="57" spans="1:35" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="13" t="s">
-        <v>57</v>
-      </c>
+      <c r="V56" s="19"/>
+      <c r="W56" s="19"/>
+      <c r="X56" s="19"/>
+      <c r="Y56" s="19"/>
+      <c r="Z56" s="19"/>
+      <c r="AA56" s="28"/>
+      <c r="AB56" s="28"/>
+      <c r="AC56" s="28"/>
+      <c r="AD56" s="28"/>
+      <c r="AE56" s="28"/>
+      <c r="AF56" s="28"/>
+      <c r="AG56" s="28"/>
+    </row>
+    <row r="57" spans="1:35" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A57" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B57">
+        <v>15</v>
+      </c>
+      <c r="C57">
+        <v>1</v>
+      </c>
+      <c r="D57">
+        <v>15</v>
+      </c>
+      <c r="E57">
+        <v>1</v>
+      </c>
+      <c r="F57" t="s">
+        <v>58</v>
+      </c>
+      <c r="U57" s="35"/>
+      <c r="X57" s="19"/>
+      <c r="Y57" s="19"/>
+      <c r="Z57" s="19"/>
+      <c r="AA57" s="19"/>
+      <c r="AB57" s="19"/>
+      <c r="AC57" s="19"/>
+      <c r="AD57" s="19"/>
+      <c r="AE57" s="28"/>
+      <c r="AF57" s="28"/>
+      <c r="AG57" s="22"/>
     </row>
     <row r="58" spans="1:35" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A58" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B58">
         <v>15</v>
       </c>
       <c r="C58">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D58">
+        <v>15</v>
+      </c>
+      <c r="E58">
+        <v>2</v>
+      </c>
+      <c r="F58" t="s">
+        <v>58</v>
+      </c>
+      <c r="U58" s="35"/>
+      <c r="V58" s="31"/>
+      <c r="AD58" s="19"/>
+      <c r="AE58" s="19"/>
+      <c r="AF58" s="19"/>
+      <c r="AG58" s="22"/>
+      <c r="AH58" s="22"/>
+    </row>
+    <row r="59" spans="1:35" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A59" s="13" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="60" spans="1:35" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A60" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B60">
+        <v>15</v>
+      </c>
+      <c r="C60">
+        <v>2</v>
+      </c>
+      <c r="D60">
         <v>16</v>
       </c>
-      <c r="E58">
-        <v>1</v>
-      </c>
-      <c r="F58" s="24">
+      <c r="E60">
+        <v>1</v>
+      </c>
+      <c r="F60" s="24">
         <v>0.5</v>
       </c>
-      <c r="U58" s="14"/>
-      <c r="V58" s="31"/>
-      <c r="AH58" s="23"/>
-      <c r="AI58" s="23"/>
-    </row>
-    <row r="59" spans="1:35" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="5" t="s">
+      <c r="U60" s="14"/>
+      <c r="V60" s="31"/>
+      <c r="AH60" s="23"/>
+      <c r="AI60" s="23"/>
+    </row>
+    <row r="61" spans="1:35" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A61" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B59">
+      <c r="B61">
         <v>16</v>
       </c>
-      <c r="C59">
-        <v>1</v>
-      </c>
-      <c r="D59">
+      <c r="C61">
+        <v>1</v>
+      </c>
+      <c r="D61">
         <v>17</v>
       </c>
-      <c r="E59">
-        <v>1</v>
-      </c>
-      <c r="F59" s="24">
+      <c r="E61">
+        <v>1</v>
+      </c>
+      <c r="F61" s="24">
         <v>0.5</v>
       </c>
-      <c r="V59" s="14"/>
-      <c r="W59" s="31"/>
-      <c r="AI59" s="23"/>
-    </row>
-    <row r="60" spans="1:35" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+      <c r="V61" s="14"/>
+      <c r="W61" s="31"/>
+      <c r="AI61" s="23"/>
+    </row>
+    <row r="62" spans="1:35" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A62" s="13" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="63" spans="1:35" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A63" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C63" t="s">
+        <v>78</v>
+      </c>
+      <c r="F63" s="24"/>
+    </row>
+    <row r="64" spans="1:35" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A64" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C64" t="s">
+        <v>78</v>
+      </c>
+      <c r="F64" s="24"/>
+    </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="AG6:AI6"/>
+    <mergeCell ref="AG7:AI7"/>
+    <mergeCell ref="AG8:AI8"/>
+    <mergeCell ref="AG9:AI9"/>
+    <mergeCell ref="AD6:AF6"/>
+    <mergeCell ref="AD8:AF8"/>
+    <mergeCell ref="AD7:AF7"/>
+    <mergeCell ref="AE9:AF9"/>
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="G1:AI1"/>
     <mergeCell ref="A1:A2"/>
@@ -2613,14 +2686,6 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="E1:E2"/>
     <mergeCell ref="F1:F2"/>
-    <mergeCell ref="AG6:AI6"/>
-    <mergeCell ref="AG7:AI7"/>
-    <mergeCell ref="AG8:AI8"/>
-    <mergeCell ref="AG9:AI9"/>
-    <mergeCell ref="AD6:AF6"/>
-    <mergeCell ref="AD8:AF8"/>
-    <mergeCell ref="AD7:AF7"/>
-    <mergeCell ref="AE9:AF9"/>
   </mergeCells>
   <conditionalFormatting sqref="G2:BN3">
     <cfRule type="expression" dxfId="0" priority="1">

</xml_diff>

<commit_message>
New Finalised Update to Gantt Chart
</commit_message>
<xml_diff>
--- a/Gantt chart.xlsx
+++ b/Gantt chart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avaiv\software-tech-ass\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D2E4CB3-A036-49C6-9182-554978B9A8D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAE95E0C-7DBD-433C-A1B0-3307D54B3E91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28935" yWindow="-1650" windowWidth="29070" windowHeight="15750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-1635" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="74">
   <si>
     <t>ACTIVITY</t>
   </si>
@@ -266,21 +266,6 @@
   </si>
   <si>
     <t>Prepare a User Manual</t>
-  </si>
-  <si>
-    <t>Data Analysis and Reporting</t>
-  </si>
-  <si>
-    <t>Perform Data Analysis over a 12 month period</t>
-  </si>
-  <si>
-    <t>Create an Executive Summary</t>
-  </si>
-  <si>
-    <t>12 Months</t>
-  </si>
-  <si>
-    <t>Ongoing</t>
   </si>
 </sst>
 </file>
@@ -802,7 +787,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -911,6 +896,48 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="17" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="3" xfId="17" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" xfId="19" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" xfId="20">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" xfId="21">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="18" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="17" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="10" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" xfId="11" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" xfId="9" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="2" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" xfId="10" applyFill="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="2" xfId="10" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="5" xfId="10" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="22" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -919,51 +946,6 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="22" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="10" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" xfId="11" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" xfId="9" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="2" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" xfId="10" applyFill="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="2" xfId="10" applyFill="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="5" xfId="10" applyFill="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="17" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="3" xfId="17" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" xfId="19" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" xfId="20">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" xfId="21">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" xfId="22">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="18" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="17" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="23">
@@ -1260,10 +1242,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BN64"/>
+  <dimension ref="A1:BN62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="N76" sqref="N76"/>
+    <sheetView tabSelected="1" zoomScale="49" zoomScaleNormal="49" workbookViewId="0">
+      <selection activeCell="AN80" sqref="AN80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1278,55 +1260,55 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:66" x14ac:dyDescent="0.3">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="43" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="43" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="43" t="s">
+      <c r="B1" s="47" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="47" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="43" t="s">
+      <c r="E1" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="45" t="s">
+      <c r="F1" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="40" t="s">
+      <c r="G1" s="44" t="s">
         <v>58</v>
       </c>
-      <c r="H1" s="40"/>
-      <c r="I1" s="40"/>
-      <c r="J1" s="40"/>
-      <c r="K1" s="40"/>
-      <c r="L1" s="40"/>
-      <c r="M1" s="40"/>
-      <c r="N1" s="40"/>
-      <c r="O1" s="40"/>
-      <c r="P1" s="40"/>
-      <c r="Q1" s="40"/>
-      <c r="R1" s="40"/>
-      <c r="S1" s="40"/>
-      <c r="T1" s="40"/>
-      <c r="U1" s="40"/>
-      <c r="V1" s="40"/>
-      <c r="W1" s="40"/>
-      <c r="X1" s="40"/>
-      <c r="Y1" s="40"/>
-      <c r="Z1" s="40"/>
-      <c r="AA1" s="40"/>
-      <c r="AB1" s="40"/>
-      <c r="AC1" s="40"/>
-      <c r="AD1" s="40"/>
-      <c r="AE1" s="40"/>
-      <c r="AF1" s="40"/>
-      <c r="AG1" s="40"/>
-      <c r="AH1" s="40"/>
-      <c r="AI1" s="40"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
+      <c r="K1" s="44"/>
+      <c r="L1" s="44"/>
+      <c r="M1" s="44"/>
+      <c r="N1" s="44"/>
+      <c r="O1" s="44"/>
+      <c r="P1" s="44"/>
+      <c r="Q1" s="44"/>
+      <c r="R1" s="44"/>
+      <c r="S1" s="44"/>
+      <c r="T1" s="44"/>
+      <c r="U1" s="44"/>
+      <c r="V1" s="44"/>
+      <c r="W1" s="44"/>
+      <c r="X1" s="44"/>
+      <c r="Y1" s="44"/>
+      <c r="Z1" s="44"/>
+      <c r="AA1" s="44"/>
+      <c r="AB1" s="44"/>
+      <c r="AC1" s="44"/>
+      <c r="AD1" s="44"/>
+      <c r="AE1" s="44"/>
+      <c r="AF1" s="44"/>
+      <c r="AG1" s="44"/>
+      <c r="AH1" s="44"/>
+      <c r="AI1" s="44"/>
       <c r="AJ1" s="2"/>
       <c r="AK1" s="2"/>
       <c r="AL1" s="2"/>
@@ -1360,12 +1342,12 @@
       <c r="BN1" s="2"/>
     </row>
     <row r="2" spans="1:66" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="42"/>
-      <c r="B2" s="44"/>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
+      <c r="A2" s="46"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
       <c r="G2" s="22">
         <v>1</v>
       </c>
@@ -1489,12 +1471,12 @@
       <c r="A3" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="B3" s="39" t="s">
+      <c r="B3" s="43" t="s">
         <v>58</v>
       </c>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
       <c r="F3" s="9"/>
       <c r="G3" s="8"/>
       <c r="H3" s="1"/>
@@ -1628,32 +1610,32 @@
       <c r="H6" s="24"/>
       <c r="I6" s="25"/>
       <c r="AC6" s="31"/>
-      <c r="AD6" s="36" t="s">
+      <c r="AD6" s="50" t="s">
         <v>61</v>
       </c>
-      <c r="AE6" s="37"/>
-      <c r="AF6" s="38"/>
-      <c r="AG6" s="36" t="s">
+      <c r="AE6" s="51"/>
+      <c r="AF6" s="52"/>
+      <c r="AG6" s="50" t="s">
         <v>64</v>
       </c>
-      <c r="AH6" s="37"/>
-      <c r="AI6" s="38"/>
+      <c r="AH6" s="51"/>
+      <c r="AI6" s="52"/>
     </row>
     <row r="7" spans="1:66" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="11" t="s">
         <v>50</v>
       </c>
       <c r="AC7" s="32"/>
-      <c r="AD7" s="36" t="s">
+      <c r="AD7" s="50" t="s">
         <v>60</v>
       </c>
-      <c r="AE7" s="37"/>
-      <c r="AF7" s="38"/>
-      <c r="AG7" s="36" t="s">
+      <c r="AE7" s="51"/>
+      <c r="AF7" s="52"/>
+      <c r="AG7" s="50" t="s">
         <v>65</v>
       </c>
-      <c r="AH7" s="37"/>
-      <c r="AI7" s="38"/>
+      <c r="AH7" s="51"/>
+      <c r="AI7" s="52"/>
     </row>
     <row r="8" spans="1:66" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
@@ -1678,16 +1660,16 @@
       <c r="I8" s="23"/>
       <c r="J8" s="23"/>
       <c r="AC8" s="33"/>
-      <c r="AD8" s="36" t="s">
+      <c r="AD8" s="50" t="s">
         <v>62</v>
       </c>
-      <c r="AE8" s="37"/>
-      <c r="AF8" s="38"/>
-      <c r="AG8" s="36" t="s">
+      <c r="AE8" s="51"/>
+      <c r="AF8" s="52"/>
+      <c r="AG8" s="50" t="s">
         <v>66</v>
       </c>
-      <c r="AH8" s="37"/>
-      <c r="AI8" s="38"/>
+      <c r="AH8" s="51"/>
+      <c r="AI8" s="52"/>
     </row>
     <row r="9" spans="1:66" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
@@ -1712,15 +1694,15 @@
       <c r="K9" s="25"/>
       <c r="AC9" s="32"/>
       <c r="AD9" s="31"/>
-      <c r="AE9" s="36" t="s">
+      <c r="AE9" s="50" t="s">
         <v>63</v>
       </c>
-      <c r="AF9" s="38"/>
-      <c r="AG9" s="36" t="s">
+      <c r="AF9" s="52"/>
+      <c r="AG9" s="50" t="s">
         <v>67</v>
       </c>
-      <c r="AH9" s="37"/>
-      <c r="AI9" s="38"/>
+      <c r="AH9" s="51"/>
+      <c r="AI9" s="52"/>
     </row>
     <row r="10" spans="1:66" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
@@ -2067,7 +2049,7 @@
       <c r="F28" s="19">
         <v>1</v>
       </c>
-      <c r="N28" s="52"/>
+      <c r="N28" s="41"/>
       <c r="O28" s="25"/>
       <c r="P28" s="25"/>
       <c r="Q28" s="25"/>
@@ -2075,7 +2057,7 @@
       <c r="S28" s="25"/>
       <c r="T28" s="25"/>
       <c r="U28" s="25"/>
-      <c r="V28" s="46"/>
+      <c r="V28" s="36"/>
     </row>
     <row r="29" spans="1:28" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
@@ -2096,15 +2078,15 @@
       <c r="F29" s="19">
         <v>1</v>
       </c>
-      <c r="O29" s="52"/>
-      <c r="P29" s="52"/>
+      <c r="O29" s="41"/>
+      <c r="P29" s="41"/>
       <c r="Q29" s="25"/>
       <c r="R29" s="25"/>
       <c r="S29" s="25"/>
       <c r="T29" s="25"/>
       <c r="U29" s="25"/>
-      <c r="V29" s="47"/>
-      <c r="W29" s="46"/>
+      <c r="V29" s="37"/>
+      <c r="W29" s="36"/>
     </row>
     <row r="30" spans="1:28" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
@@ -2125,17 +2107,17 @@
       <c r="F30" s="19">
         <v>1</v>
       </c>
-      <c r="P30" s="52"/>
-      <c r="Q30" s="52"/>
-      <c r="R30" s="52"/>
+      <c r="P30" s="41"/>
+      <c r="Q30" s="41"/>
+      <c r="R30" s="41"/>
       <c r="S30" s="25"/>
       <c r="T30" s="25"/>
       <c r="U30" s="25"/>
       <c r="V30" s="25"/>
       <c r="W30" s="25"/>
-      <c r="X30" s="46"/>
-      <c r="Y30" s="46"/>
-      <c r="Z30" s="46"/>
+      <c r="X30" s="36"/>
+      <c r="Y30" s="36"/>
+      <c r="Z30" s="36"/>
     </row>
     <row r="31" spans="1:28" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
@@ -2156,18 +2138,18 @@
       <c r="F31" s="19">
         <v>1</v>
       </c>
-      <c r="Q31" s="52"/>
-      <c r="R31" s="52"/>
-      <c r="S31" s="52"/>
-      <c r="T31" s="52"/>
+      <c r="Q31" s="41"/>
+      <c r="R31" s="41"/>
+      <c r="S31" s="41"/>
+      <c r="T31" s="41"/>
       <c r="U31" s="25"/>
       <c r="V31" s="25"/>
       <c r="W31" s="25"/>
       <c r="X31" s="25"/>
-      <c r="Y31" s="46"/>
-      <c r="Z31" s="46"/>
-      <c r="AA31" s="46"/>
-      <c r="AB31" s="46"/>
+      <c r="Y31" s="36"/>
+      <c r="Z31" s="36"/>
+      <c r="AA31" s="36"/>
+      <c r="AB31" s="36"/>
     </row>
     <row r="32" spans="1:28" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="3" t="s">
@@ -2188,16 +2170,16 @@
       <c r="F32" s="19">
         <v>1</v>
       </c>
-      <c r="S32" s="52"/>
-      <c r="T32" s="52"/>
+      <c r="S32" s="41"/>
+      <c r="T32" s="41"/>
       <c r="U32" s="25"/>
       <c r="V32" s="25"/>
       <c r="W32" s="25"/>
       <c r="X32" s="25"/>
       <c r="Y32" s="25"/>
       <c r="Z32" s="25"/>
-      <c r="AA32" s="46"/>
-      <c r="AB32" s="46"/>
+      <c r="AA32" s="36"/>
+      <c r="AB32" s="36"/>
     </row>
     <row r="33" spans="1:32" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="3" t="s">
@@ -2220,7 +2202,7 @@
       </c>
       <c r="S33" s="16"/>
       <c r="T33" s="16"/>
-      <c r="U33" s="52"/>
+      <c r="U33" s="41"/>
       <c r="V33" s="25"/>
       <c r="W33" s="25"/>
       <c r="X33" s="25"/>
@@ -2228,7 +2210,7 @@
       <c r="Z33" s="25"/>
       <c r="AA33" s="25"/>
       <c r="AB33" s="25"/>
-      <c r="AC33" s="46"/>
+      <c r="AC33" s="36"/>
     </row>
     <row r="34" spans="1:32" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="21" t="s">
@@ -2254,7 +2236,7 @@
       <c r="F35" s="19">
         <v>1</v>
       </c>
-      <c r="O35" s="52"/>
+      <c r="O35" s="41"/>
       <c r="P35" s="25"/>
       <c r="Q35" s="25"/>
       <c r="R35" s="25"/>
@@ -2262,7 +2244,7 @@
       <c r="T35" s="25"/>
       <c r="U35" s="25"/>
       <c r="V35" s="25"/>
-      <c r="W35" s="46"/>
+      <c r="W35" s="36"/>
     </row>
     <row r="36" spans="1:32" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="3" t="s">
@@ -2283,16 +2265,16 @@
       <c r="F36" s="19">
         <v>1</v>
       </c>
-      <c r="P36" s="52"/>
-      <c r="Q36" s="52"/>
+      <c r="P36" s="41"/>
+      <c r="Q36" s="41"/>
       <c r="R36" s="25"/>
       <c r="S36" s="25"/>
       <c r="T36" s="25"/>
       <c r="U36" s="25"/>
       <c r="V36" s="25"/>
       <c r="W36" s="25"/>
-      <c r="X36" s="46"/>
-      <c r="Y36" s="46"/>
+      <c r="X36" s="36"/>
+      <c r="Y36" s="36"/>
     </row>
     <row r="37" spans="1:32" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="s">
@@ -2313,16 +2295,16 @@
       <c r="F37" s="19">
         <v>1</v>
       </c>
-      <c r="Q37" s="52"/>
-      <c r="R37" s="52"/>
+      <c r="Q37" s="41"/>
+      <c r="R37" s="41"/>
       <c r="S37" s="25"/>
       <c r="T37" s="25"/>
       <c r="U37" s="25"/>
       <c r="V37" s="25"/>
       <c r="W37" s="25"/>
       <c r="X37" s="25"/>
-      <c r="Y37" s="46"/>
-      <c r="Z37" s="46"/>
+      <c r="Y37" s="36"/>
+      <c r="Z37" s="36"/>
     </row>
     <row r="38" spans="1:32" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="3" t="s">
@@ -2343,17 +2325,17 @@
       <c r="F38" s="19">
         <v>1</v>
       </c>
-      <c r="Q38" s="52"/>
-      <c r="R38" s="52"/>
-      <c r="S38" s="52"/>
+      <c r="Q38" s="41"/>
+      <c r="R38" s="41"/>
+      <c r="S38" s="41"/>
       <c r="T38" s="25"/>
       <c r="U38" s="25"/>
       <c r="V38" s="25"/>
       <c r="W38" s="25"/>
       <c r="X38" s="25"/>
-      <c r="Y38" s="46"/>
-      <c r="Z38" s="46"/>
-      <c r="AA38" s="46"/>
+      <c r="Y38" s="36"/>
+      <c r="Z38" s="36"/>
+      <c r="AA38" s="36"/>
     </row>
     <row r="39" spans="1:32" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="3" t="s">
@@ -2374,16 +2356,16 @@
       <c r="F39" s="19">
         <v>1</v>
       </c>
-      <c r="S39" s="52"/>
-      <c r="T39" s="52"/>
+      <c r="S39" s="41"/>
+      <c r="T39" s="41"/>
       <c r="U39" s="25"/>
       <c r="V39" s="25"/>
       <c r="W39" s="25"/>
       <c r="X39" s="25"/>
       <c r="Y39" s="25"/>
       <c r="Z39" s="25"/>
-      <c r="AA39" s="46"/>
-      <c r="AB39" s="46"/>
+      <c r="AA39" s="36"/>
+      <c r="AB39" s="36"/>
     </row>
     <row r="40" spans="1:32" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="3" t="s">
@@ -2404,19 +2386,19 @@
       <c r="F40" s="19">
         <v>1</v>
       </c>
-      <c r="R40" s="52"/>
-      <c r="S40" s="52"/>
-      <c r="T40" s="52"/>
-      <c r="U40" s="52"/>
+      <c r="R40" s="41"/>
+      <c r="S40" s="41"/>
+      <c r="T40" s="41"/>
+      <c r="U40" s="41"/>
       <c r="V40" s="25"/>
       <c r="W40" s="25"/>
       <c r="X40" s="25"/>
       <c r="Y40" s="25"/>
-      <c r="Z40" s="46"/>
-      <c r="AA40" s="46"/>
-      <c r="AB40" s="46"/>
-      <c r="AC40" s="46"/>
-      <c r="AD40" s="53"/>
+      <c r="Z40" s="36"/>
+      <c r="AA40" s="36"/>
+      <c r="AB40" s="36"/>
+      <c r="AC40" s="36"/>
+      <c r="AD40" s="42"/>
     </row>
     <row r="41" spans="1:32" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="13" t="s">
@@ -2442,16 +2424,16 @@
       <c r="F42" s="19">
         <v>1</v>
       </c>
-      <c r="T42" s="48"/>
-      <c r="U42" s="48"/>
-      <c r="V42" s="48"/>
+      <c r="T42" s="38"/>
+      <c r="U42" s="38"/>
+      <c r="V42" s="38"/>
       <c r="W42" s="25"/>
       <c r="X42" s="25"/>
       <c r="Y42" s="25"/>
       <c r="Z42" s="25"/>
-      <c r="AA42" s="49"/>
-      <c r="AB42" s="49"/>
-      <c r="AC42" s="49"/>
+      <c r="AA42" s="39"/>
+      <c r="AB42" s="39"/>
+      <c r="AC42" s="39"/>
     </row>
     <row r="43" spans="1:32" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="3" t="s">
@@ -2472,14 +2454,14 @@
       <c r="F43" s="19">
         <v>1</v>
       </c>
-      <c r="V43" s="48"/>
+      <c r="V43" s="38"/>
       <c r="W43" s="25"/>
       <c r="X43" s="25"/>
       <c r="Y43" s="25"/>
       <c r="Z43" s="25"/>
       <c r="AA43" s="25"/>
       <c r="AB43" s="25"/>
-      <c r="AC43" s="49"/>
+      <c r="AC43" s="39"/>
     </row>
     <row r="44" spans="1:32" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="3" t="s">
@@ -2500,15 +2482,15 @@
       <c r="F44" s="19">
         <v>1</v>
       </c>
-      <c r="V44" s="48"/>
-      <c r="W44" s="48"/>
+      <c r="V44" s="38"/>
+      <c r="W44" s="38"/>
       <c r="X44" s="25"/>
       <c r="Y44" s="25"/>
       <c r="Z44" s="25"/>
       <c r="AA44" s="25"/>
       <c r="AB44" s="25"/>
-      <c r="AC44" s="49"/>
-      <c r="AD44" s="49"/>
+      <c r="AC44" s="39"/>
+      <c r="AD44" s="39"/>
     </row>
     <row r="45" spans="1:32" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="3" t="s">
@@ -2529,14 +2511,14 @@
       <c r="F45" s="19">
         <v>1</v>
       </c>
-      <c r="X45" s="48"/>
+      <c r="X45" s="38"/>
       <c r="Y45" s="25"/>
       <c r="Z45" s="25"/>
       <c r="AA45" s="25"/>
       <c r="AB45" s="25"/>
       <c r="AC45" s="25"/>
       <c r="AD45" s="25"/>
-      <c r="AE45" s="49"/>
+      <c r="AE45" s="39"/>
     </row>
     <row r="46" spans="1:32" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="35" t="s">
@@ -2557,14 +2539,14 @@
       <c r="F46" s="19">
         <v>1</v>
       </c>
-      <c r="Y46" s="48"/>
+      <c r="Y46" s="38"/>
       <c r="Z46" s="25"/>
       <c r="AA46" s="25"/>
       <c r="AB46" s="25"/>
       <c r="AC46" s="25"/>
       <c r="AD46" s="25"/>
       <c r="AE46" s="25"/>
-      <c r="AF46" s="49"/>
+      <c r="AF46" s="39"/>
     </row>
     <row r="47" spans="1:32" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="13" t="s">
@@ -2608,18 +2590,18 @@
       <c r="P48" s="17"/>
       <c r="Q48" s="17"/>
       <c r="R48" s="17"/>
-      <c r="S48" s="50"/>
-      <c r="T48" s="50"/>
-      <c r="U48" s="50"/>
-      <c r="V48" s="50"/>
-      <c r="W48" s="50"/>
-      <c r="X48" s="50"/>
-      <c r="Y48" s="50"/>
-      <c r="Z48" s="50"/>
-      <c r="AA48" s="50"/>
-      <c r="AB48" s="50"/>
-      <c r="AC48" s="50"/>
-      <c r="AD48" s="50"/>
+      <c r="S48" s="40"/>
+      <c r="T48" s="40"/>
+      <c r="U48" s="40"/>
+      <c r="V48" s="40"/>
+      <c r="W48" s="40"/>
+      <c r="X48" s="40"/>
+      <c r="Y48" s="40"/>
+      <c r="Z48" s="40"/>
+      <c r="AA48" s="40"/>
+      <c r="AB48" s="40"/>
+      <c r="AC48" s="40"/>
+      <c r="AD48" s="40"/>
       <c r="AE48" s="16"/>
     </row>
     <row r="49" spans="1:35" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -2646,16 +2628,16 @@
       <c r="P49" s="16"/>
       <c r="Q49" s="16"/>
       <c r="R49" s="16"/>
-      <c r="W49" s="50"/>
-      <c r="X49" s="50"/>
-      <c r="Y49" s="50"/>
-      <c r="Z49" s="50"/>
-      <c r="AA49" s="50"/>
-      <c r="AB49" s="50"/>
-      <c r="AC49" s="50"/>
-      <c r="AD49" s="50"/>
-      <c r="AE49" s="50"/>
-      <c r="AF49" s="50"/>
+      <c r="W49" s="40"/>
+      <c r="X49" s="40"/>
+      <c r="Y49" s="40"/>
+      <c r="Z49" s="40"/>
+      <c r="AA49" s="40"/>
+      <c r="AB49" s="40"/>
+      <c r="AC49" s="40"/>
+      <c r="AD49" s="40"/>
+      <c r="AE49" s="40"/>
+      <c r="AF49" s="40"/>
     </row>
     <row r="50" spans="1:35" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
@@ -2683,14 +2665,14 @@
       <c r="R50" s="16"/>
       <c r="X50" s="16"/>
       <c r="Y50" s="16"/>
-      <c r="Z50" s="50"/>
-      <c r="AA50" s="50"/>
-      <c r="AB50" s="50"/>
-      <c r="AC50" s="50"/>
-      <c r="AD50" s="50"/>
-      <c r="AE50" s="50"/>
-      <c r="AF50" s="50"/>
-      <c r="AG50" s="50"/>
+      <c r="Z50" s="40"/>
+      <c r="AA50" s="40"/>
+      <c r="AB50" s="40"/>
+      <c r="AC50" s="40"/>
+      <c r="AD50" s="40"/>
+      <c r="AE50" s="40"/>
+      <c r="AF50" s="40"/>
+      <c r="AG50" s="40"/>
     </row>
     <row r="51" spans="1:35" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" s="5" t="s">
@@ -2711,8 +2693,8 @@
       <c r="F51" s="19">
         <v>1</v>
       </c>
-      <c r="AC51" s="50"/>
-      <c r="AH51" s="50"/>
+      <c r="AC51" s="40"/>
+      <c r="AH51" s="40"/>
     </row>
     <row r="52" spans="1:35" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A52" s="13" t="s">
@@ -3002,39 +2984,17 @@
       <c r="AH61" s="25"/>
       <c r="AI61" s="18"/>
     </row>
-    <row r="62" spans="1:35" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A62" s="13" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="63" spans="1:35" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A63" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="C63" t="s">
-        <v>77</v>
-      </c>
-      <c r="F63" s="19" t="s">
-        <v>78</v>
-      </c>
-      <c r="AH63" s="51"/>
-      <c r="AI63" s="51"/>
-    </row>
-    <row r="64" spans="1:35" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A64" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="C64" t="s">
-        <v>77</v>
-      </c>
-      <c r="F64" s="19" t="s">
-        <v>78</v>
-      </c>
-      <c r="AH64" s="51"/>
-      <c r="AI64" s="51"/>
-    </row>
+    <row r="62" spans="1:35" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="AG6:AI6"/>
+    <mergeCell ref="AG7:AI7"/>
+    <mergeCell ref="AG8:AI8"/>
+    <mergeCell ref="AG9:AI9"/>
+    <mergeCell ref="AD6:AF6"/>
+    <mergeCell ref="AD8:AF8"/>
+    <mergeCell ref="AD7:AF7"/>
+    <mergeCell ref="AE9:AF9"/>
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="G1:AI1"/>
     <mergeCell ref="A1:A2"/>
@@ -3043,14 +3003,6 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="E1:E2"/>
     <mergeCell ref="F1:F2"/>
-    <mergeCell ref="AG6:AI6"/>
-    <mergeCell ref="AG7:AI7"/>
-    <mergeCell ref="AG8:AI8"/>
-    <mergeCell ref="AG9:AI9"/>
-    <mergeCell ref="AD6:AF6"/>
-    <mergeCell ref="AD8:AF8"/>
-    <mergeCell ref="AD7:AF7"/>
-    <mergeCell ref="AE9:AF9"/>
   </mergeCells>
   <conditionalFormatting sqref="G2:BN3">
     <cfRule type="expression" dxfId="0" priority="1">

</xml_diff>